<commit_message>
AC-90. WSO Issuer ID UI validation.
Excel sheet locked.
WSOIssuerID validation added to grid.
WSOIssuerID inclusion in refData.
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -2,19 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Desktop\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B7DB517-B60C-47CA-8854-74338C9CF196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9136F52-09F8-4CAB-84C3-D4ACE4F21857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="O73qSt8rIAnQVCLsFA7lUn21XTa36Pt7GIQmqPn8YT1W12J4E5Vvept8cpK9MaBGqTVtsSfUV1h+ej2oUwBopQ==" workbookSaltValue="g3CxC7+oLZ3yGbWfTTplIQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="223">
   <si>
     <t>Issuer Short Name(optional)</t>
   </si>
@@ -695,6 +696,15 @@
   </si>
   <si>
     <t>JPY</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
   </si>
 </sst>
 </file>
@@ -722,12 +732,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -738,8 +742,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -760,17 +770,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -857,36 +856,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,10 +1206,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AF4C19-D9D8-4D17-BA71-C91E169BA22D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:XFD11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <pane xSplit="1" topLeftCell="XEQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1216,58 +1221,94 @@
     <col min="4" max="16384" width="9.1796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:1 16370:16384" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:1 16370:16384" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:1 16370:16384" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:1 16370:16384" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:1 16370:16384" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:1 16370:16384" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:1 16370:16384" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:1 16370:16384" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:1 16370:16384" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:1 16370:16384" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>56</v>
       </c>
+      <c r="XEP10"/>
+      <c r="XEQ10"/>
+      <c r="XER10"/>
+      <c r="XES10"/>
+      <c r="XET10"/>
+      <c r="XEU10"/>
+      <c r="XEV10"/>
+      <c r="XEW10"/>
+      <c r="XEX10"/>
+      <c r="XEY10"/>
+      <c r="XEZ10"/>
+      <c r="XFA10"/>
+      <c r="XFB10"/>
+      <c r="XFC10"/>
+      <c r="XFD10"/>
+    </row>
+    <row r="11" spans="1:1 16370:16384" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="XEP11"/>
+      <c r="XEQ11"/>
+      <c r="XER11"/>
+      <c r="XES11"/>
+      <c r="XET11"/>
+      <c r="XEU11"/>
+      <c r="XEV11"/>
+      <c r="XEW11"/>
+      <c r="XEX11"/>
+      <c r="XEY11"/>
+      <c r="XEZ11"/>
+      <c r="XFA11"/>
+      <c r="XFB11"/>
+      <c r="XFC11"/>
+      <c r="XFD11"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <sheetProtection algorithmName="SHA-512" hashValue="ITMxt1gHuHTdhxjirZXO83ny1APU6+J2i0uFyX5B1hyORbTZ3K6Ji8bCiDbBzWfKfx29C24yz4BE1nP+rrtotA==" saltValue="rYG7GfzCmVIcGk9EqMZJqw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="3">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:XFD3" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
     </dataValidation>
@@ -1275,12 +1316,15 @@
       <formula1>-99999999999999</formula1>
       <formula2>99999999999999</formula2>
     </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:XFD7" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
+      <formula1>0</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{270CF3BB-5B9B-40EC-8A02-7CFFCB3B95C5}">
           <x14:formula1>
             <xm:f>Sheet2!$G$1:$G$5</xm:f>
@@ -1305,17 +1349,11 @@
           </x14:formula1>
           <xm:sqref>B5:XFD5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CA0AD2C-0AF4-4BD4-9B65-21E28E153E4A}">
           <x14:formula1>
-            <xm:f>Sheet2!$D$1:$D$185</xm:f>
+            <xm:f>Sheet2!$H$1:$H$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:XFD7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6DEF0870-2B3E-4A7C-A73E-A2C9E047F4DC}">
-          <x14:formula1>
-            <xm:f>Sheet2!$E$1:$E$185</xm:f>
-          </x14:formula1>
-          <xm:sqref>A8:XFD8</xm:sqref>
+          <xm:sqref>B11:XFD11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1326,10 +1364,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE38E7C1-F75A-461B-83D8-D3E941B09876}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G185"/>
+  <dimension ref="A1:H185"/>
   <sheetViews>
-    <sheetView topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1341,7 +1379,7 @@
     <col min="5" max="5" width="44.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1357,11 +1395,14 @@
       <c r="E1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="12" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1377,11 +1418,14 @@
       <c r="E2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="12" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1397,11 +1441,11 @@
       <c r="E3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1415,11 +1459,11 @@
       <c r="E4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="12" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1433,11 +1477,11 @@
       <c r="E5" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="12" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1452,7 +1496,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1465,7 +1509,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1478,7 +1522,7 @@
         <v>871668</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1491,7 +1535,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -1504,7 +1548,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1517,7 +1561,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1530,7 +1574,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1543,7 +1587,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1556,7 +1600,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1569,7 +1613,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
AC-90. Action col removed from Excel
WSOIssuerID validation added for investment, income subtypes.
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E8D18C-F1B5-4969-80B8-838D722F9A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37D7AB8-383F-497D-A1E5-F26BA3416D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="lsI402VvOK1r/BeViKpM6VtBNldQDSQUMjf/Uu9QTc7dE7ixDxbNMGSytydWJvHRhOnYJaW63qlfh14H121Vkw==" workbookSaltValue="XYB/AhtrzFNa44IUW+Nq3w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="222">
   <si>
     <t>Issuer Short Name(optional)</t>
   </si>
@@ -696,9 +696,6 @@
   </si>
   <si>
     <t>JPY</t>
-  </si>
-  <si>
-    <t>Action</t>
   </si>
   <si>
     <t>ADD</t>
@@ -714,10 +711,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -856,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -887,7 +891,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1264,17 +1269,13 @@
       </c>
     </row>
     <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>220</v>
-      </c>
-    </row>
+    <row r="11" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="HNfL0Qc+3XnBteQSb6A/cXcnU2r9tii2PpD1oIdsjkqQUICSPH7Af4z90q/wZnju5b3TDzjsTCXo/1wNzeZSvg==" saltValue="bS7U/mCAN5KCgaFYB7zbNw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="3">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:XFD3" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1366,7 +1367,7 @@
         <v>215</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1389,7 +1390,7 @@
         <v>218</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
AC-139. Excel template modified.
Capital type/subtype categories added.
IssuerID binded to single capital activity.
Reload grid on bulk update.
IssuerID validation in range added.
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,8 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37D7AB8-383F-497D-A1E5-F26BA3416D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="lsI402VvOK1r/BeViKpM6VtBNldQDSQUMjf/Uu9QTc7dE7ixDxbNMGSytydWJvHRhOnYJaW63qlfh14H121Vkw==" workbookSaltValue="XYB/AhtrzFNa44IUW+Nq3w==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDB82D3-1B67-4045-93A8-BFDC29F57954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="227">
   <si>
     <t>Issuer Short Name(optional)</t>
   </si>
@@ -176,15 +175,6 @@
     <t>SMA Q</t>
   </si>
   <si>
-    <t xml:space="preserve">Distribution </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contribution </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recallable distribution </t>
-  </si>
-  <si>
     <t>Hedging Costs</t>
   </si>
   <si>
@@ -194,9 +184,6 @@
     <t>Investment</t>
   </si>
   <si>
-    <t xml:space="preserve">Partnership expenses </t>
-  </si>
-  <si>
     <t>Realised Gain</t>
   </si>
   <si>
@@ -698,10 +685,37 @@
     <t>JPY</t>
   </si>
   <si>
-    <t>ADD</t>
-  </si>
-  <si>
-    <t>UPDATE</t>
+    <t>Contribution</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Recallable distribution</t>
+  </si>
+  <si>
+    <t>NAV</t>
+  </si>
+  <si>
+    <t>Prior distribution</t>
+  </si>
+  <si>
+    <t>Partnership expenses</t>
+  </si>
+  <si>
+    <t>NAV Adjustment</t>
+  </si>
+  <si>
+    <t>Management Fee</t>
+  </si>
+  <si>
+    <t>Performance Fee</t>
+  </si>
+  <si>
+    <t>Other Expenses</t>
+  </si>
+  <si>
+    <t>FX Gain &amp; Loss</t>
   </si>
 </sst>
 </file>
@@ -860,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -893,6 +907,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1225,12 +1240,12 @@
   <sheetData>
     <row r="1" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -1265,17 +1280,17 @@
     </row>
     <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HNfL0Qc+3XnBteQSb6A/cXcnU2r9tii2PpD1oIdsjkqQUICSPH7Af4z90q/wZnju5b3TDzjsTCXo/1wNzeZSvg==" saltValue="bS7U/mCAN5KCgaFYB7zbNw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="3">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:XFD3" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1307,13 +1322,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD33D8DB-60D7-4F0B-971A-5F8F33CA4B56}">
           <x14:formula1>
-            <xm:f>Sheet2!$B$1:$B$3</xm:f>
+            <xm:f>Sheet2!$B$1:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>B4:XFD4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$6</xm:f>
+            <xm:f>Sheet2!$C$1:$C$12</xm:f>
           </x14:formula1>
           <xm:sqref>B5:XFD5</xm:sqref>
         </x14:dataValidation>
@@ -1335,7 +1350,7 @@
   <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1352,101 +1367,101 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>216</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1">
         <v>21</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>220</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>217</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2">
         <v>22</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>221</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D3" s="2">
         <v>26</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>219</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2">
         <v>29</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>220</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>221</v>
       </c>
       <c r="D5" s="2">
         <v>48</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1455,13 +1470,13 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2">
         <v>70</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1469,12 +1484,14 @@
         <v>12</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>219</v>
+      </c>
       <c r="D7" s="2">
         <v>71</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1482,7 +1499,9 @@
         <v>13</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="D8" s="2">
         <v>72</v>
       </c>
@@ -1495,12 +1514,14 @@
         <v>14</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="D9" s="2">
         <v>74</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1508,12 +1529,14 @@
         <v>15</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="D10" s="2">
         <v>77</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1521,7 +1544,9 @@
         <v>16</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="D11" s="2">
         <v>83</v>
       </c>
@@ -1534,7 +1559,9 @@
         <v>17</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>226</v>
+      </c>
       <c r="D12" s="2">
         <v>92</v>
       </c>
@@ -1565,7 +1592,7 @@
         <v>129</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1578,7 +1605,7 @@
         <v>130</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1591,7 +1618,7 @@
         <v>141</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1604,7 +1631,7 @@
         <v>142</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1617,7 +1644,7 @@
         <v>148</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1630,7 +1657,7 @@
         <v>158</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1643,7 +1670,7 @@
         <v>176</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1656,7 +1683,7 @@
         <v>181</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1669,7 +1696,7 @@
         <v>182</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1682,7 +1709,7 @@
         <v>183</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1695,7 +1722,7 @@
         <v>200</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1708,7 +1735,7 @@
         <v>202</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1721,7 +1748,7 @@
         <v>205</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1734,7 +1761,7 @@
         <v>206</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1747,7 +1774,7 @@
         <v>208</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1760,7 +1787,7 @@
         <v>215</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1773,7 +1800,7 @@
         <v>216</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1786,7 +1813,7 @@
         <v>218</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1799,7 +1826,7 @@
         <v>219</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1812,7 +1839,7 @@
         <v>220</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1825,7 +1852,7 @@
         <v>221</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1838,7 +1865,7 @@
         <v>228</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1851,7 +1878,7 @@
         <v>232</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1864,7 +1891,7 @@
         <v>249</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1877,7 +1904,7 @@
         <v>254</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1890,7 +1917,7 @@
         <v>261</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1903,7 +1930,7 @@
         <v>277</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1914,7 +1941,7 @@
         <v>287</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1925,7 +1952,7 @@
         <v>291</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1936,7 +1963,7 @@
         <v>304</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -1947,7 +1974,7 @@
         <v>315</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1958,7 +1985,7 @@
         <v>317</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -1969,7 +1996,7 @@
         <v>346</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1980,7 +2007,7 @@
         <v>350</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -1991,7 +2018,7 @@
         <v>353</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -2002,7 +2029,7 @@
         <v>354</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -2013,7 +2040,7 @@
         <v>366</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -2024,7 +2051,7 @@
         <v>381</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -2035,7 +2062,7 @@
         <v>382</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -2046,7 +2073,7 @@
         <v>387</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -2057,7 +2084,7 @@
         <v>396</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -2068,7 +2095,7 @@
         <v>397</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -2079,7 +2106,7 @@
         <v>401</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -2090,7 +2117,7 @@
         <v>411</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
@@ -2101,7 +2128,7 @@
         <v>419</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
@@ -2112,7 +2139,7 @@
         <v>421</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
@@ -2123,7 +2150,7 @@
         <v>429</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
@@ -2134,7 +2161,7 @@
         <v>432</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -2145,7 +2172,7 @@
         <v>441</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -2156,7 +2183,7 @@
         <v>446</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -2167,7 +2194,7 @@
         <v>447</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -2178,7 +2205,7 @@
         <v>449</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
@@ -2189,7 +2216,7 @@
         <v>451</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
@@ -2200,7 +2227,7 @@
         <v>456</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -2211,7 +2238,7 @@
         <v>458</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -2222,7 +2249,7 @@
         <v>459</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -2233,7 +2260,7 @@
         <v>460</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -2244,7 +2271,7 @@
         <v>464</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -2255,7 +2282,7 @@
         <v>466</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -2266,7 +2293,7 @@
         <v>469</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
@@ -2277,7 +2304,7 @@
         <v>472</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -2288,7 +2315,7 @@
         <v>477</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -2299,7 +2326,7 @@
         <v>479</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
@@ -2310,7 +2337,7 @@
         <v>480</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -2321,7 +2348,7 @@
         <v>485</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -2332,7 +2359,7 @@
         <v>486</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -2343,7 +2370,7 @@
         <v>492</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
@@ -2354,7 +2381,7 @@
         <v>494</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
@@ -2365,7 +2392,7 @@
         <v>506</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -2376,7 +2403,7 @@
         <v>510</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
@@ -2387,7 +2414,7 @@
         <v>514</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
@@ -2398,7 +2425,7 @@
         <v>523</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
@@ -2409,7 +2436,7 @@
         <v>524</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
@@ -2420,7 +2447,7 @@
         <v>532</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
@@ -2431,7 +2458,7 @@
         <v>554</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -2442,7 +2469,7 @@
         <v>555</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
@@ -2453,7 +2480,7 @@
         <v>574</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
@@ -2464,7 +2491,7 @@
         <v>578</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
@@ -2475,7 +2502,7 @@
         <v>579</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
@@ -2486,7 +2513,7 @@
         <v>580</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
@@ -2497,7 +2524,7 @@
         <v>581</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
@@ -2508,7 +2535,7 @@
         <v>582</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
@@ -2519,7 +2546,7 @@
         <v>584</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
@@ -2530,7 +2557,7 @@
         <v>589</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
@@ -2541,7 +2568,7 @@
         <v>594</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
@@ -2552,7 +2579,7 @@
         <v>595</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
@@ -2563,7 +2590,7 @@
         <v>596</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
@@ -2574,7 +2601,7 @@
         <v>601</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
@@ -2585,7 +2612,7 @@
         <v>603</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
@@ -2596,7 +2623,7 @@
         <v>604</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
@@ -2607,7 +2634,7 @@
         <v>605</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
@@ -2618,7 +2645,7 @@
         <v>607</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
@@ -2629,7 +2656,7 @@
         <v>631</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
@@ -2640,7 +2667,7 @@
         <v>632</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
@@ -2651,7 +2678,7 @@
         <v>766</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
@@ -2662,7 +2689,7 @@
         <v>790</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
@@ -2673,7 +2700,7 @@
         <v>805</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
@@ -2684,7 +2711,7 @@
         <v>810</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
@@ -2695,7 +2722,7 @@
         <v>811</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
@@ -2706,7 +2733,7 @@
         <v>812</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
@@ -2717,7 +2744,7 @@
         <v>813</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
@@ -2728,7 +2755,7 @@
         <v>814</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
@@ -2739,7 +2766,7 @@
         <v>815</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
@@ -2750,7 +2777,7 @@
         <v>816</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
@@ -2761,7 +2788,7 @@
         <v>817</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
@@ -2772,7 +2799,7 @@
         <v>818</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
@@ -2783,7 +2810,7 @@
         <v>819</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
@@ -2794,7 +2821,7 @@
         <v>820</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
@@ -2805,7 +2832,7 @@
         <v>821</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
@@ -2816,7 +2843,7 @@
         <v>822</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
@@ -2827,7 +2854,7 @@
         <v>823</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
@@ -2838,7 +2865,7 @@
         <v>824</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
@@ -2849,7 +2876,7 @@
         <v>825</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
@@ -2860,7 +2887,7 @@
         <v>826</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
@@ -2871,7 +2898,7 @@
         <v>827</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
@@ -2882,7 +2909,7 @@
         <v>828</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
@@ -2893,7 +2920,7 @@
         <v>829</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
@@ -2904,7 +2931,7 @@
         <v>830</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
@@ -2915,7 +2942,7 @@
         <v>831</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
@@ -2926,7 +2953,7 @@
         <v>832</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
@@ -2937,7 +2964,7 @@
         <v>833</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
@@ -2948,7 +2975,7 @@
         <v>834</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
@@ -2959,7 +2986,7 @@
         <v>835</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
@@ -2970,7 +2997,7 @@
         <v>836</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
@@ -2981,7 +3008,7 @@
         <v>837</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
@@ -2992,7 +3019,7 @@
         <v>838</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
@@ -3003,7 +3030,7 @@
         <v>839</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
@@ -3014,7 +3041,7 @@
         <v>840</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
@@ -3025,7 +3052,7 @@
         <v>841</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
@@ -3036,7 +3063,7 @@
         <v>842</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
@@ -3047,7 +3074,7 @@
         <v>843</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
@@ -3058,7 +3085,7 @@
         <v>844</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
@@ -3069,7 +3096,7 @@
         <v>845</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
@@ -3080,7 +3107,7 @@
         <v>846</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
@@ -3091,7 +3118,7 @@
         <v>847</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
@@ -3102,7 +3129,7 @@
         <v>848</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
@@ -3113,7 +3140,7 @@
         <v>849</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
@@ -3124,7 +3151,7 @@
         <v>850</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
@@ -3135,7 +3162,7 @@
         <v>851</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
@@ -3146,7 +3173,7 @@
         <v>852</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
@@ -3157,7 +3184,7 @@
         <v>853</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
@@ -3168,7 +3195,7 @@
         <v>854</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
@@ -3179,7 +3206,7 @@
         <v>855</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
@@ -3190,7 +3217,7 @@
         <v>856</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
@@ -3201,7 +3228,7 @@
         <v>857</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
@@ -3212,7 +3239,7 @@
         <v>858</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
@@ -3223,7 +3250,7 @@
         <v>859</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
@@ -3234,7 +3261,7 @@
         <v>860</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
@@ -3245,7 +3272,7 @@
         <v>861</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
@@ -3256,7 +3283,7 @@
         <v>862</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
@@ -3267,7 +3294,7 @@
         <v>863</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
@@ -3278,7 +3305,7 @@
         <v>864</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
@@ -3289,7 +3316,7 @@
         <v>865</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
@@ -3300,7 +3327,7 @@
         <v>866</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
@@ -3311,7 +3338,7 @@
         <v>867</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
@@ -3322,7 +3349,7 @@
         <v>868</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
@@ -3333,7 +3360,7 @@
         <v>869</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
@@ -3344,7 +3371,7 @@
         <v>870</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
@@ -3355,7 +3382,7 @@
         <v>871</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
@@ -3366,7 +3393,7 @@
         <v>872</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
@@ -3377,7 +3404,7 @@
         <v>873</v>
       </c>
       <c r="E174" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
@@ -3388,7 +3415,7 @@
         <v>874</v>
       </c>
       <c r="E175" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
@@ -3399,7 +3426,7 @@
         <v>875</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
@@ -3410,7 +3437,7 @@
         <v>876</v>
       </c>
       <c r="E177" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
@@ -3421,7 +3448,7 @@
         <v>877</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
@@ -3432,7 +3459,7 @@
         <v>878</v>
       </c>
       <c r="E179" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
@@ -3443,7 +3470,7 @@
         <v>879</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.35">
@@ -3454,7 +3481,7 @@
         <v>880</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.35">
@@ -3465,7 +3492,7 @@
         <v>881</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
@@ -3476,7 +3503,7 @@
         <v>882</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
@@ -3487,7 +3514,7 @@
         <v>883</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.35">
@@ -3498,7 +3525,7 @@
         <v>884</v>
       </c>
       <c r="E185" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AC- 142 template updated
call date added
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skumar\source\ArkRepo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDB82D3-1B67-4045-93A8-BFDC29F57954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AF3F00-CFB3-4FCA-99D9-BD7AC1F86CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="227">
-  <si>
-    <t>Issuer Short Name(optional)</t>
-  </si>
-  <si>
-    <t>Wso Issuer ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="230">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -52,9 +46,6 @@
     <t>Capital Subtype</t>
   </si>
   <si>
-    <t>Amount (fund ccy)</t>
-  </si>
-  <si>
     <t>CS1FEUR</t>
   </si>
   <si>
@@ -716,6 +707,24 @@
   </si>
   <si>
     <t>FX Gain &amp; Loss</t>
+  </si>
+  <si>
+    <t>Call Date</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Wso Asset ID</t>
+  </si>
+  <si>
+    <t>Position Currency</t>
+  </si>
+  <si>
+    <t>GIR (Pos - Fund ccy)</t>
+  </si>
+  <si>
+    <t>Arrangement Fee</t>
   </si>
 </sst>
 </file>
@@ -1223,83 +1232,99 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AF4C19-D9D8-4D17-BA71-C91E169BA22D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="11"/>
+    <col min="1" max="1" width="33.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <dataValidations count="3">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:XFD3" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
+  <sheetProtection algorithmName="SHA-512" hashValue="t+1x4StNHlwdEb73Dq5wc9o1Gd+EqL1pC0q7s44PcBA4gTceeDwE429BYzuhh1cRmcppNO6S7cxUs2SAR8VWLw==" saltValue="6IxM0G1XGCphNX1EruKMyA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="5">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:XFD1" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:XFD6" xr:uid="{E26CAB39-A4D5-4CDD-A869-59535BC6FDF5}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:XFD7" xr:uid="{E26CAB39-A4D5-4CDD-A869-59535BC6FDF5}">
       <formula1>-99999999999999</formula1>
       <formula2>99999999999999</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:XFD7" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:XFD10" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:XFD2" xr:uid="{820604F4-ED75-4A4C-AC98-FF2036A48C8C}">
+      <formula1>40909</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:XFD6" xr:uid="{01C54EDB-8CDE-4226-AD78-37C83EDB08F0}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1312,31 +1337,31 @@
           <x14:formula1>
             <xm:f>Sheet2!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:XFD2</xm:sqref>
+          <xm:sqref>B4:XFD5 B7:XFD7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5921C6A4-2CD9-4EAE-9809-BA84C4675AA1}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:XFD1</xm:sqref>
+          <xm:sqref>B3:XFD3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD33D8DB-60D7-4F0B-971A-5F8F33CA4B56}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B4:XFD4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
-          <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5:XFD5</xm:sqref>
+          <xm:sqref>B8:XFD8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CA0AD2C-0AF4-4BD4-9B65-21E28E153E4A}">
           <x14:formula1>
             <xm:f>Sheet2!$H$1:$H$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B11:XFD11</xm:sqref>
+          <xm:sqref>B13:XFD13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
+          <x14:formula1>
+            <xm:f>Sheet2!$C$1:$C$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9:XFD9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1347,160 +1372,160 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE38E7C1-F75A-461B-83D8-D3E941B09876}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H185"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1">
         <v>21</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2">
         <v>22</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2">
         <v>26</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2">
         <v>29</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D5" s="2">
         <v>48</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2">
         <v>70</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D7" s="2">
         <v>71</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D8" s="2">
         <v>72</v>
@@ -1509,43 +1534,43 @@
         <v>871668</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D9" s="2">
         <v>74</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D10" s="2">
         <v>77</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D11" s="2">
         <v>83</v>
@@ -1554,13 +1579,13 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D12" s="2">
         <v>92</v>
@@ -1569,12 +1594,14 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="D13" s="2">
         <v>100</v>
       </c>
@@ -1582,9 +1609,9 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1592,12 +1619,12 @@
         <v>129</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1605,12 +1632,12 @@
         <v>130</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1618,12 +1645,12 @@
         <v>141</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1631,12 +1658,12 @@
         <v>142</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1644,12 +1671,12 @@
         <v>148</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1657,12 +1684,12 @@
         <v>158</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1670,12 +1697,12 @@
         <v>176</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1683,12 +1710,12 @@
         <v>181</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1696,12 +1723,12 @@
         <v>182</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1709,12 +1736,12 @@
         <v>183</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1722,12 +1749,12 @@
         <v>200</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1735,12 +1762,12 @@
         <v>202</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1748,12 +1775,12 @@
         <v>205</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1761,12 +1788,12 @@
         <v>206</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1774,12 +1801,12 @@
         <v>208</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1787,12 +1814,12 @@
         <v>215</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1800,12 +1827,12 @@
         <v>216</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1813,12 +1840,12 @@
         <v>218</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1826,12 +1853,12 @@
         <v>219</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1839,12 +1866,12 @@
         <v>220</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1852,12 +1879,12 @@
         <v>221</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1865,12 +1892,12 @@
         <v>228</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1878,12 +1905,12 @@
         <v>232</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1891,12 +1918,12 @@
         <v>249</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1904,12 +1931,12 @@
         <v>254</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1917,12 +1944,12 @@
         <v>261</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1930,10 +1957,10 @@
         <v>277</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1941,10 +1968,10 @@
         <v>287</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1952,10 +1979,10 @@
         <v>291</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1963,10 +1990,10 @@
         <v>304</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1974,10 +2001,10 @@
         <v>315</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1985,10 +2012,10 @@
         <v>317</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1996,10 +2023,10 @@
         <v>346</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2007,10 +2034,10 @@
         <v>350</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2018,10 +2045,10 @@
         <v>353</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2029,10 +2056,10 @@
         <v>354</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2040,10 +2067,10 @@
         <v>366</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2051,10 +2078,10 @@
         <v>381</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2062,10 +2089,10 @@
         <v>382</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2073,10 +2100,10 @@
         <v>387</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2084,10 +2111,10 @@
         <v>396</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2095,10 +2122,10 @@
         <v>397</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2106,10 +2133,10 @@
         <v>401</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2117,10 +2144,10 @@
         <v>411</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2128,10 +2155,10 @@
         <v>419</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2139,10 +2166,10 @@
         <v>421</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2150,10 +2177,10 @@
         <v>429</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2161,10 +2188,10 @@
         <v>432</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2172,10 +2199,10 @@
         <v>441</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2183,10 +2210,10 @@
         <v>446</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2194,10 +2221,10 @@
         <v>447</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2205,10 +2232,10 @@
         <v>449</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2216,10 +2243,10 @@
         <v>451</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2227,10 +2254,10 @@
         <v>456</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2238,10 +2265,10 @@
         <v>458</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2249,10 +2276,10 @@
         <v>459</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2260,10 +2287,10 @@
         <v>460</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2271,10 +2298,10 @@
         <v>464</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2282,10 +2309,10 @@
         <v>466</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2293,10 +2320,10 @@
         <v>469</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2304,10 +2331,10 @@
         <v>472</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2315,10 +2342,10 @@
         <v>477</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2326,10 +2353,10 @@
         <v>479</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2337,10 +2364,10 @@
         <v>480</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2348,10 +2375,10 @@
         <v>485</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2359,10 +2386,10 @@
         <v>486</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2370,10 +2397,10 @@
         <v>492</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2381,10 +2408,10 @@
         <v>494</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2392,10 +2419,10 @@
         <v>506</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2403,10 +2430,10 @@
         <v>510</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2414,10 +2441,10 @@
         <v>514</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2425,10 +2452,10 @@
         <v>523</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2436,10 +2463,10 @@
         <v>524</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2447,10 +2474,10 @@
         <v>532</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2458,10 +2485,10 @@
         <v>554</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2469,10 +2496,10 @@
         <v>555</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2480,10 +2507,10 @@
         <v>574</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2491,10 +2518,10 @@
         <v>578</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2502,10 +2529,10 @@
         <v>579</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2513,10 +2540,10 @@
         <v>580</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2524,10 +2551,10 @@
         <v>581</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2535,10 +2562,10 @@
         <v>582</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2546,10 +2573,10 @@
         <v>584</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2557,10 +2584,10 @@
         <v>589</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2568,10 +2595,10 @@
         <v>594</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2579,10 +2606,10 @@
         <v>595</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2590,10 +2617,10 @@
         <v>596</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2601,10 +2628,10 @@
         <v>601</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2612,10 +2639,10 @@
         <v>603</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2623,10 +2650,10 @@
         <v>604</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2634,10 +2661,10 @@
         <v>605</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2645,10 +2672,10 @@
         <v>607</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2656,10 +2683,10 @@
         <v>631</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2667,10 +2694,10 @@
         <v>632</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2678,10 +2705,10 @@
         <v>766</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2689,10 +2716,10 @@
         <v>790</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2700,10 +2727,10 @@
         <v>805</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2711,10 +2738,10 @@
         <v>810</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2722,10 +2749,10 @@
         <v>811</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2733,10 +2760,10 @@
         <v>812</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2744,10 +2771,10 @@
         <v>813</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2755,10 +2782,10 @@
         <v>814</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2766,10 +2793,10 @@
         <v>815</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2777,10 +2804,10 @@
         <v>816</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2788,10 +2815,10 @@
         <v>817</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2799,10 +2826,10 @@
         <v>818</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2810,10 +2837,10 @@
         <v>819</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -2821,10 +2848,10 @@
         <v>820</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -2832,10 +2859,10 @@
         <v>821</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -2843,10 +2870,10 @@
         <v>822</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -2854,10 +2881,10 @@
         <v>823</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -2865,10 +2892,10 @@
         <v>824</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -2876,10 +2903,10 @@
         <v>825</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -2887,10 +2914,10 @@
         <v>826</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -2898,10 +2925,10 @@
         <v>827</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -2909,10 +2936,10 @@
         <v>828</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -2920,10 +2947,10 @@
         <v>829</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -2931,10 +2958,10 @@
         <v>830</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -2942,10 +2969,10 @@
         <v>831</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -2953,10 +2980,10 @@
         <v>832</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -2964,10 +2991,10 @@
         <v>833</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -2975,10 +3002,10 @@
         <v>834</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -2986,10 +3013,10 @@
         <v>835</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -2997,10 +3024,10 @@
         <v>836</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3008,10 +3035,10 @@
         <v>837</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3019,10 +3046,10 @@
         <v>838</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3030,10 +3057,10 @@
         <v>839</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3041,10 +3068,10 @@
         <v>840</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3052,10 +3079,10 @@
         <v>841</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3063,10 +3090,10 @@
         <v>842</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3074,10 +3101,10 @@
         <v>843</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3085,10 +3112,10 @@
         <v>844</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3096,10 +3123,10 @@
         <v>845</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3107,10 +3134,10 @@
         <v>846</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3118,10 +3145,10 @@
         <v>847</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3129,10 +3156,10 @@
         <v>848</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3140,10 +3167,10 @@
         <v>849</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3151,10 +3178,10 @@
         <v>850</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3162,10 +3189,10 @@
         <v>851</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3173,10 +3200,10 @@
         <v>852</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3184,10 +3211,10 @@
         <v>853</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3195,10 +3222,10 @@
         <v>854</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3206,10 +3233,10 @@
         <v>855</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3217,10 +3244,10 @@
         <v>856</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3228,10 +3255,10 @@
         <v>857</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3239,10 +3266,10 @@
         <v>858</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3250,10 +3277,10 @@
         <v>859</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3261,10 +3288,10 @@
         <v>860</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3272,10 +3299,10 @@
         <v>861</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3283,10 +3310,10 @@
         <v>862</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3294,10 +3321,10 @@
         <v>863</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3305,10 +3332,10 @@
         <v>864</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3316,10 +3343,10 @@
         <v>865</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3327,10 +3354,10 @@
         <v>866</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3338,10 +3365,10 @@
         <v>867</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3349,10 +3376,10 @@
         <v>868</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3360,10 +3387,10 @@
         <v>869</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3371,10 +3398,10 @@
         <v>870</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3382,10 +3409,10 @@
         <v>871</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3393,10 +3420,10 @@
         <v>872</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3404,10 +3431,10 @@
         <v>873</v>
       </c>
       <c r="E174" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3415,10 +3442,10 @@
         <v>874</v>
       </c>
       <c r="E175" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3426,10 +3453,10 @@
         <v>875</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3437,10 +3464,10 @@
         <v>876</v>
       </c>
       <c r="E177" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3448,10 +3475,10 @@
         <v>877</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3459,10 +3486,10 @@
         <v>878</v>
       </c>
       <c r="E179" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3470,10 +3497,10 @@
         <v>879</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3481,10 +3508,10 @@
         <v>880</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3492,10 +3519,10 @@
         <v>881</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3503,10 +3530,10 @@
         <v>882</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3514,21 +3541,28 @@
         <v>883</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
-      <c r="C185" s="8"/>
+      <c r="C185" s="2"/>
       <c r="D185" s="8">
         <v>884</v>
       </c>
       <c r="E185" s="9" t="s">
-        <v>66</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C186" s="8"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="NVpRpO87HqZTiHvnJwMZ+GxeADBA3/uvIS+eoQVTuVno3Pzx8CYzFq2FWE59aQ5OYMl/QwnoOGPMuujZOP0yMQ==" saltValue="ezL04WNl6NEq80oBB7OCGA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C9:C10">
+    <sortCondition ref="C9:C10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
AC-142. GIR, AssetID, posCcy validation added to bulk update.
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skumar\source\ArkRepo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AF3F00-CFB3-4FCA-99D9-BD7AC1F86CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DFB22D-9CC6-4D61-8C12-C7E3BA4BEF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="231">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -725,6 +725,9 @@
   </si>
   <si>
     <t>Arrangement Fee</t>
+  </si>
+  <si>
+    <t>Rebates</t>
   </si>
 </sst>
 </file>
@@ -1236,80 +1239,81 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B9" sqref="B9"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" style="10" customWidth="1"/>
     <col min="2" max="2" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="11"/>
+    <col min="3" max="3" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="t+1x4StNHlwdEb73Dq5wc9o1Gd+EqL1pC0q7s44PcBA4gTceeDwE429BYzuhh1cRmcppNO6S7cxUs2SAR8VWLw==" saltValue="6IxM0G1XGCphNX1EruKMyA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="V8hI+CDI/XTAFA1+GFShP1DWOR6chBCHA9Z7vtKf28Rc4KVC/GzCzAvc0hNQPZ0cPIcSS3ptzMv3k6ZKC9ruKg==" saltValue="eNJlbZ+IG4dcuJIGeOeeLg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:XFD1" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1359,7 +1363,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$13</xm:f>
+            <xm:f>Sheet2!$C$1:$C$14</xm:f>
           </x14:formula1>
           <xm:sqref>B9:XFD9</xm:sqref>
         </x14:dataValidation>
@@ -1375,19 +1379,19 @@
   <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1408,7 +1412,7 @@
       </c>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1429,7 +1433,7 @@
       </c>
       <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1449,7 +1453,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1469,7 +1473,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1489,7 +1493,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1519,7 +1523,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>871668</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1549,7 +1553,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1564,7 +1568,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1579,7 +1583,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1594,7 +1598,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1609,12 +1613,14 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="D14" s="2">
         <v>129</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1648,7 +1654,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -1674,7 +1680,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -1687,7 +1693,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1700,7 +1706,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -1713,7 +1719,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -1739,7 +1745,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -1752,7 +1758,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
@@ -1791,7 +1797,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
@@ -1817,7 +1823,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
@@ -1830,7 +1836,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
@@ -1856,7 +1862,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -1882,7 +1888,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1921,7 +1927,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
@@ -1934,7 +1940,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -1947,7 +1953,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
@@ -1960,7 +1966,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1971,7 +1977,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1982,7 +1988,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1993,7 +1999,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2004,7 +2010,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2015,7 +2021,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2026,7 +2032,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2037,7 +2043,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2048,7 +2054,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2059,7 +2065,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2070,7 +2076,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2081,7 +2087,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2092,7 +2098,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2103,7 +2109,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2114,7 +2120,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2125,7 +2131,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2136,7 +2142,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2147,7 +2153,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2158,7 +2164,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2169,7 +2175,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2180,7 +2186,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2191,7 +2197,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2202,7 +2208,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2213,7 +2219,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2224,7 +2230,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2235,7 +2241,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2246,7 +2252,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2257,7 +2263,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2268,7 +2274,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2279,7 +2285,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2290,7 +2296,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2301,7 +2307,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2312,7 +2318,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2323,7 +2329,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2334,7 +2340,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2345,7 +2351,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2356,7 +2362,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2367,7 +2373,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2378,7 +2384,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2389,7 +2395,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2400,7 +2406,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2411,7 +2417,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2422,7 +2428,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2433,7 +2439,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2444,7 +2450,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2455,7 +2461,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2466,7 +2472,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2477,7 +2483,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2488,7 +2494,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2499,7 +2505,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2510,7 +2516,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2521,7 +2527,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2532,7 +2538,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2543,7 +2549,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2554,7 +2560,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2565,7 +2571,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2576,7 +2582,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2587,7 +2593,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2598,7 +2604,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2609,7 +2615,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2620,7 +2626,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2631,7 +2637,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2642,7 +2648,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2653,7 +2659,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2664,7 +2670,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2675,7 +2681,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2686,7 +2692,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2697,7 +2703,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2708,7 +2714,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2719,7 +2725,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2730,7 +2736,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2741,7 +2747,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2752,7 +2758,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2763,7 +2769,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2774,7 +2780,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2785,7 +2791,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2796,7 +2802,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2807,7 +2813,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2818,7 +2824,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2829,7 +2835,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2840,7 +2846,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -2851,7 +2857,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -2862,7 +2868,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -2873,7 +2879,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -2884,7 +2890,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -2895,7 +2901,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -2906,7 +2912,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -2917,7 +2923,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -2928,7 +2934,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -2939,7 +2945,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -2950,7 +2956,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -2961,7 +2967,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -2972,7 +2978,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -2983,7 +2989,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -2994,7 +3000,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3005,7 +3011,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3016,7 +3022,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3027,7 +3033,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3038,7 +3044,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3049,7 +3055,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3060,7 +3066,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3071,7 +3077,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3082,7 +3088,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3093,7 +3099,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3104,7 +3110,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3115,7 +3121,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3126,7 +3132,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3137,7 +3143,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3148,7 +3154,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3159,7 +3165,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3170,7 +3176,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3181,7 +3187,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3192,7 +3198,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3203,7 +3209,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3214,7 +3220,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3225,7 +3231,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3236,7 +3242,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3247,7 +3253,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3258,7 +3264,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3269,7 +3275,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3280,7 +3286,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3291,7 +3297,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3302,7 +3308,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3313,7 +3319,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3324,7 +3330,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3335,7 +3341,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3346,7 +3352,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3357,7 +3363,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3368,7 +3374,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3379,7 +3385,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3390,7 +3396,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3401,7 +3407,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3412,7 +3418,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3423,7 +3429,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3434,7 +3440,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3445,7 +3451,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3456,7 +3462,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3467,7 +3473,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3478,7 +3484,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3489,7 +3495,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3500,7 +3506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3511,7 +3517,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3522,7 +3528,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3533,7 +3539,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3544,7 +3550,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="2"/>
@@ -3555,11 +3561,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C186" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NVpRpO87HqZTiHvnJwMZ+GxeADBA3/uvIS+eoQVTuVno3Pzx8CYzFq2FWE59aQ5OYMl/QwnoOGPMuujZOP0yMQ==" saltValue="ezL04WNl6NEq80oBB7OCGA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="q86acTZAS0l80Iw2XZXS9dnBbZCjrv5hMIg+mNBypNoBLYLxqiP2dVyqiTb1Usm2AhaKbyG1fcGOczP2gtu73A==" saltValue="6z4fyGsMW4jK8JbSWSpKbg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C9:C10">
     <sortCondition ref="C9:C10"/>
   </sortState>

</xml_diff>

<commit_message>
AC-139  ccy added for pos ccy in CA bulk upload template
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skumar\source\ArkRepo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DFB22D-9CC6-4D61-8C12-C7E3BA4BEF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6369082A-46DF-4A52-9847-4EB9EF73E342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="236">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -728,6 +728,21 @@
   </si>
   <si>
     <t>Rebates</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEK </t>
   </si>
 </sst>
 </file>
@@ -886,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -920,6 +935,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1239,81 +1255,81 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="11"/>
+    <col min="3" max="3" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="V8hI+CDI/XTAFA1+GFShP1DWOR6chBCHA9Z7vtKf28Rc4KVC/GzCzAvc0hNQPZ0cPIcSS3ptzMv3k6ZKC9ruKg==" saltValue="eNJlbZ+IG4dcuJIGeOeeLg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="XqeHUEzh+dyHP9uUApM1BZusiPZVmm7iLwiYSuPqCgvL6a176n3EBzSW8w8Fw9znuR6gXJtJHdSOm6UA4w26BQ==" saltValue="Jnk2HtyEQHMKBBcNB3BZPw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:XFD1" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1336,12 +1352,12 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{270CF3BB-5B9B-40EC-8A02-7CFFCB3B95C5}">
           <x14:formula1>
             <xm:f>Sheet2!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B4:XFD5 B7:XFD7</xm:sqref>
+          <xm:sqref>B7:XFD7 XEF4:XFD4 B4:XEE4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5921C6A4-2CD9-4EAE-9809-BA84C4675AA1}">
           <x14:formula1>
@@ -1367,6 +1383,12 @@
           </x14:formula1>
           <xm:sqref>B9:XFD9</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85863E50-D527-4AC5-A2D8-C6D4BC7E5ACE}">
+          <x14:formula1>
+            <xm:f>Sheet2!$I$1:$I$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:XFD5</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1376,22 +1398,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE38E7C1-F75A-461B-83D8-D3E941B09876}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H186"/>
+  <dimension ref="A1:I186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1408,11 +1431,14 @@
         <v>79</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1429,11 +1455,14 @@
         <v>80</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H2" s="20"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1450,10 +1479,13 @@
         <v>81</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1470,10 +1502,13 @@
         <v>82</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1490,10 +1525,13 @@
         <v>83</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1507,8 +1545,11 @@
       <c r="E6" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1522,8 +1563,11 @@
       <c r="E7" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1537,8 +1581,11 @@
       <c r="E8" s="6">
         <v>871668</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" s="12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1552,8 +1599,11 @@
       <c r="E9" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1567,8 +1617,11 @@
       <c r="E10" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1583,7 +1636,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1598,7 +1651,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1613,7 +1666,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1628,7 +1681,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1641,7 +1694,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1654,7 +1707,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1667,7 +1720,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -1680,7 +1733,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -1693,7 +1746,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1706,7 +1759,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -1719,7 +1772,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -1732,7 +1785,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -1745,7 +1798,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -1758,7 +1811,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -1771,7 +1824,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -1784,7 +1837,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
@@ -1797,7 +1850,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -1810,7 +1863,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
@@ -1823,7 +1876,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
@@ -1836,7 +1889,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
@@ -1849,7 +1902,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
@@ -1862,7 +1915,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -1875,7 +1928,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -1888,7 +1941,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
@@ -1901,7 +1954,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
@@ -1914,7 +1967,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1927,7 +1980,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
@@ -1940,7 +1993,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -1953,7 +2006,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
@@ -1966,7 +2019,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1977,7 +2030,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1988,7 +2041,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1999,7 +2052,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2010,7 +2063,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2021,7 +2074,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2032,7 +2085,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2043,7 +2096,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2054,7 +2107,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2065,7 +2118,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2076,7 +2129,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2087,7 +2140,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2098,7 +2151,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2109,7 +2162,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2120,7 +2173,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2131,7 +2184,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2142,7 +2195,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2153,7 +2206,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2164,7 +2217,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2175,7 +2228,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2186,7 +2239,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2197,7 +2250,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2208,7 +2261,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2219,7 +2272,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2230,7 +2283,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2241,7 +2294,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2252,7 +2305,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2263,7 +2316,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2274,7 +2327,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2285,7 +2338,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2296,7 +2349,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2307,7 +2360,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2318,7 +2371,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2329,7 +2382,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2340,7 +2393,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2351,7 +2404,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2362,7 +2415,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2373,7 +2426,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2384,7 +2437,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2395,7 +2448,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2406,7 +2459,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2417,7 +2470,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2428,7 +2481,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2439,7 +2492,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2450,7 +2503,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2461,7 +2514,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2472,7 +2525,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2483,7 +2536,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2494,7 +2547,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2505,7 +2558,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2516,7 +2569,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2527,7 +2580,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2538,7 +2591,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2549,7 +2602,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2560,7 +2613,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2571,7 +2624,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2582,7 +2635,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2593,7 +2646,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2604,7 +2657,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2615,7 +2668,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2626,7 +2679,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2637,7 +2690,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2648,7 +2701,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2659,7 +2712,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2670,7 +2723,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2681,7 +2734,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2692,7 +2745,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2703,7 +2756,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2714,7 +2767,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2725,7 +2778,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2736,7 +2789,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2747,7 +2800,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2758,7 +2811,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2769,7 +2822,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2780,7 +2833,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2791,7 +2844,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2802,7 +2855,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2813,7 +2866,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2824,7 +2877,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2835,7 +2888,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2846,7 +2899,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -2857,7 +2910,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -2868,7 +2921,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -2879,7 +2932,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -2890,7 +2943,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -2901,7 +2954,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -2912,7 +2965,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -2923,7 +2976,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -2934,7 +2987,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -2945,7 +2998,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -2956,7 +3009,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -2967,7 +3020,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -2978,7 +3031,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -2989,7 +3042,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3000,7 +3053,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3011,7 +3064,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3022,7 +3075,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3033,7 +3086,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3044,7 +3097,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3055,7 +3108,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3066,7 +3119,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3077,7 +3130,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3088,7 +3141,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3099,7 +3152,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3110,7 +3163,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3121,7 +3174,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3132,7 +3185,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3143,7 +3196,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3154,7 +3207,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3165,7 +3218,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3176,7 +3229,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3187,7 +3240,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3198,7 +3251,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3209,7 +3262,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3220,7 +3273,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3231,7 +3284,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3242,7 +3295,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3253,7 +3306,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3264,7 +3317,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3275,7 +3328,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3286,7 +3339,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3297,7 +3350,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3308,7 +3361,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3319,7 +3372,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3330,7 +3383,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3341,7 +3394,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3352,7 +3405,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3363,7 +3416,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3374,7 +3427,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3385,7 +3438,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3396,7 +3449,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3407,7 +3460,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3418,7 +3471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3429,7 +3482,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3440,7 +3493,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3451,7 +3504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3462,7 +3515,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3473,7 +3526,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3484,7 +3537,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3495,7 +3548,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3506,7 +3559,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3517,7 +3570,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3528,7 +3581,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3539,7 +3592,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3550,7 +3603,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="2"/>
@@ -3561,13 +3614,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C186" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="q86acTZAS0l80Iw2XZXS9dnBbZCjrv5hMIg+mNBypNoBLYLxqiP2dVyqiTb1Usm2AhaKbyG1fcGOczP2gtu73A==" saltValue="6z4fyGsMW4jK8JbSWSpKbg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C9:C10">
-    <sortCondition ref="C9:C10"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ANTEf2y0LtCbUqohELCtjXr4pdZNUHzyfZfxX48GZLeMwHLRkS5OWe4nvJ6cfomoaMi90pHAxUvbIxNzE4xzqA==" saltValue="hq7p2jAMvF47ZpAcRDQe0g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G186">
+    <sortCondition ref="G1:G186"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
AC-142. Added Advanced tax distribution, Carry as subtypes
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,10 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skumar\source\ArkRepo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6369082A-46DF-4A52-9847-4EB9EF73E342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3284FE-ECEE-4319-972A-3A823F5DC5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="rvu8yHobDhBFXD3MZeKNPQxM8vo7JKyKs9nvBut/fJkf2U3B9HXEOuWMPRXcHbEGxJ0jIlYzQGANDV6jGL39zg==" workbookSaltValue="NIi125CSBbMO5IkoZZgRyg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="238">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -743,6 +744,12 @@
   </si>
   <si>
     <t xml:space="preserve">SEK </t>
+  </si>
+  <si>
+    <t>Advanced Tax Distribution</t>
+  </si>
+  <si>
+    <t>Carry</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1262,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H19" sqref="H19"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1336,7 @@
     </row>
     <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XqeHUEzh+dyHP9uUApM1BZusiPZVmm7iLwiYSuPqCgvL6a176n3EBzSW8w8Fw9znuR6gXJtJHdSOm6UA4w26BQ==" saltValue="Jnk2HtyEQHMKBBcNB3BZPw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="HIbiSPYSVLJjSt/0TF+9SSji47fH5c0YcCheoB5rXF8NLiULDcxhDeikCj9mHNyVp5ynTmkvIOHE6H9OLajGQg==" saltValue="bsewTkz78s9gq+pP5BtCZQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:XFD1" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1379,7 +1386,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$14</xm:f>
+            <xm:f>Sheet2!$C$1:$C$16</xm:f>
           </x14:formula1>
           <xm:sqref>B9:XFD9</xm:sqref>
         </x14:dataValidation>
@@ -1401,7 +1408,7 @@
   <dimension ref="A1:I186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1421,7 @@
     <col min="6" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1438,7 +1445,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1462,7 +1469,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1485,7 +1492,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1508,7 +1515,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1531,7 +1538,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1567,7 +1574,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1585,7 +1592,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1603,7 +1610,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1621,7 +1628,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1636,7 +1643,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1651,7 +1658,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1666,7 +1673,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1681,12 +1688,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="D15" s="2">
         <v>130</v>
       </c>
@@ -1694,12 +1703,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="D16" s="2">
         <v>141</v>
       </c>
@@ -1707,7 +1718,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1720,7 +1731,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -1733,7 +1744,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -1746,7 +1757,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1759,7 +1770,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -1772,7 +1783,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -1785,7 +1796,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -1798,7 +1809,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -1811,7 +1822,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -1824,7 +1835,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -1837,7 +1848,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
@@ -1850,7 +1861,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -1863,7 +1874,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
@@ -1876,7 +1887,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
@@ -1889,7 +1900,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
@@ -1902,7 +1913,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
@@ -1915,7 +1926,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -1928,7 +1939,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -1941,7 +1952,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
@@ -1954,7 +1965,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
@@ -1967,7 +1978,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1980,7 +1991,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
@@ -1993,7 +2004,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -2006,7 +2017,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
@@ -2019,7 +2030,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2030,7 +2041,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2041,7 +2052,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2052,7 +2063,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2063,7 +2074,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2074,7 +2085,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2085,7 +2096,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2096,7 +2107,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2107,7 +2118,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2118,7 +2129,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2129,7 +2140,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2140,7 +2151,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2151,7 +2162,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2162,7 +2173,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2173,7 +2184,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2184,7 +2195,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2195,7 +2206,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2206,7 +2217,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2217,7 +2228,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2228,7 +2239,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2239,7 +2250,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2250,7 +2261,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2261,7 +2272,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2272,7 +2283,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2283,7 +2294,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2294,7 +2305,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2305,7 +2316,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2316,7 +2327,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2327,7 +2338,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2338,7 +2349,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2349,7 +2360,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2360,7 +2371,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2371,7 +2382,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2382,7 +2393,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2393,7 +2404,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2404,7 +2415,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2415,7 +2426,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2426,7 +2437,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2437,7 +2448,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2448,7 +2459,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2459,7 +2470,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2470,7 +2481,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2481,7 +2492,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2492,7 +2503,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2503,7 +2514,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2514,7 +2525,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2525,7 +2536,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2536,7 +2547,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2547,7 +2558,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2558,7 +2569,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2569,7 +2580,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2580,7 +2591,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2591,7 +2602,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2602,7 +2613,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2613,7 +2624,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2624,7 +2635,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2635,7 +2646,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2646,7 +2657,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2657,7 +2668,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2668,7 +2679,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2679,7 +2690,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2690,7 +2701,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2701,7 +2712,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2712,7 +2723,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2723,7 +2734,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2734,7 +2745,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2745,7 +2756,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2756,7 +2767,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2767,7 +2778,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2778,7 +2789,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2789,7 +2800,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2800,7 +2811,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2811,7 +2822,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2822,7 +2833,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2833,7 +2844,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2844,7 +2855,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2855,7 +2866,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2866,7 +2877,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2877,7 +2888,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2888,7 +2899,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2899,7 +2910,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -2910,7 +2921,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -2921,7 +2932,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -2932,7 +2943,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -2943,7 +2954,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -2954,7 +2965,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -2965,7 +2976,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -2976,7 +2987,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -2987,7 +2998,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -2998,7 +3009,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3009,7 +3020,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3020,7 +3031,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3031,7 +3042,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3042,7 +3053,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3053,7 +3064,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3064,7 +3075,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3075,7 +3086,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3086,7 +3097,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3097,7 +3108,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3108,7 +3119,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3119,7 +3130,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="141" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3130,7 +3141,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3141,7 +3152,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3152,7 +3163,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3163,7 +3174,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3174,7 +3185,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3185,7 +3196,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3196,7 +3207,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3207,7 +3218,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3218,7 +3229,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3229,7 +3240,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3240,7 +3251,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3251,7 +3262,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3262,7 +3273,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3273,7 +3284,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3284,7 +3295,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3295,7 +3306,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3306,7 +3317,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3317,7 +3328,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="159" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3328,7 +3339,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3339,7 +3350,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3350,7 +3361,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3361,7 +3372,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3372,7 +3383,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3383,7 +3394,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3394,7 +3405,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3405,7 +3416,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3416,7 +3427,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3427,7 +3438,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3438,7 +3449,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3449,7 +3460,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="171" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3460,7 +3471,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3471,7 +3482,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3482,7 +3493,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3493,7 +3504,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="175" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3504,7 +3515,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3515,7 +3526,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="177" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3526,7 +3537,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="178" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3537,7 +3548,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3548,7 +3559,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3559,7 +3570,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="181" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3570,7 +3581,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3581,7 +3592,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="183" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3592,7 +3603,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3603,7 +3614,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="185" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="2"/>
@@ -3614,11 +3625,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="186" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C186" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ANTEf2y0LtCbUqohELCtjXr4pdZNUHzyfZfxX48GZLeMwHLRkS5OWe4nvJ6cfomoaMi90pHAxUvbIxNzE4xzqA==" saltValue="hq7p2jAMvF47ZpAcRDQe0g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6ZM3hTAdwDPMQ24jf/kwcZor1AjZ3jzLTNh2NSWTskM5eOzhWM/AiGX10pNn5MBtVdULyKtdwlUDBz0H0UwEew==" saltValue="erjZh30KLhrkeXUDQrmtYQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G186">
     <sortCondition ref="G1:G186"/>
   </sortState>

</xml_diff>

<commit_message>
AC-163. Added DL4 fund hedgings and GIR Cash adj as subtype
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3284FE-ECEE-4319-972A-3A823F5DC5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="rvu8yHobDhBFXD3MZeKNPQxM8vo7JKyKs9nvBut/fJkf2U3B9HXEOuWMPRXcHbEGxJ0jIlYzQGANDV6jGL39zg==" workbookSaltValue="NIi125CSBbMO5IkoZZgRyg==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E831DDD-DC84-4924-9480-B8BEF3847317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="YumvAZyDreJUyNoTSyPoB0UI+oG/IvavMmOjauHSsBtlFaaj/LhCFtQC5clVqHZkS0tzbWWC7hWyMW0PadZ2mw==" workbookSaltValue="ezceVuWz5ZxXMj0W4nLwDA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="250">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -750,6 +750,42 @@
   </si>
   <si>
     <t>Carry</t>
+  </si>
+  <si>
+    <t>DL410EUR</t>
+  </si>
+  <si>
+    <t>DL47EUR</t>
+  </si>
+  <si>
+    <t>DL47GBP</t>
+  </si>
+  <si>
+    <t>DL47JPY</t>
+  </si>
+  <si>
+    <t>DL47USD</t>
+  </si>
+  <si>
+    <t>DL4LEV10EUR</t>
+  </si>
+  <si>
+    <t>DL4LEV7EUR</t>
+  </si>
+  <si>
+    <t>DL4LEV7USD</t>
+  </si>
+  <si>
+    <t>DL4LEVS7EUR</t>
+  </si>
+  <si>
+    <t>DL4LEVS7USD</t>
+  </si>
+  <si>
+    <t>DL4S10EUR</t>
+  </si>
+  <si>
+    <t>GIR Cash Adj</t>
   </si>
 </sst>
 </file>
@@ -759,7 +795,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,8 +810,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,8 +843,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAEAAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -904,11 +953,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -943,6 +1007,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1265,78 +1335,78 @@
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="11"/>
+    <col min="3" max="3" width="9.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HIbiSPYSVLJjSt/0TF+9SSji47fH5c0YcCheoB5rXF8NLiULDcxhDeikCj9mHNyVp5ynTmkvIOHE6H9OLajGQg==" saltValue="bsewTkz78s9gq+pP5BtCZQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="iqZwMnPjYDjH0P2Bqi7XNo4y6NzPGrSEziiuJfqA8jsx1vjYFn5xl5RZgLrUCAaoc6YPKf6YaiBf691XOZjR5Q==" saltValue="7hHThJS7SfjEOCV8iiIAEw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:XFD1" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1368,7 +1438,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5921C6A4-2CD9-4EAE-9809-BA84C4675AA1}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$1:$A$40</xm:f>
+            <xm:f>Sheet2!$A$1:$A$51</xm:f>
           </x14:formula1>
           <xm:sqref>B3:XFD3</xm:sqref>
         </x14:dataValidation>
@@ -1386,7 +1456,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$16</xm:f>
+            <xm:f>Sheet2!$C$1:$C$17</xm:f>
           </x14:formula1>
           <xm:sqref>B9:XFD9</xm:sqref>
         </x14:dataValidation>
@@ -1407,21 +1477,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" style="21" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="21"/>
+    <col min="5" max="5" width="44.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1445,7 +1515,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1469,7 +1539,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1492,7 +1562,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1515,7 +1585,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1538,7 +1608,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1556,7 +1626,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1644,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1592,7 +1662,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1610,7 +1680,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1628,7 +1698,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1643,7 +1713,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1658,7 +1728,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1673,7 +1743,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1688,7 +1758,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1703,7 +1773,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1718,12 +1788,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>249</v>
+      </c>
       <c r="D17" s="2">
         <v>142</v>
       </c>
@@ -1731,7 +1803,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -1744,7 +1816,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -1757,7 +1829,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1770,7 +1842,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -1783,7 +1855,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -1796,7 +1868,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -1809,7 +1881,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -1822,7 +1894,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -1835,7 +1907,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -1848,7 +1920,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
@@ -1861,7 +1933,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -1874,7 +1946,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
@@ -1887,7 +1959,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
@@ -1900,7 +1972,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
@@ -1913,7 +1985,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
@@ -1926,7 +1998,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -1939,7 +2011,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -1952,7 +2024,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
@@ -1965,7 +2037,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
@@ -1978,7 +2050,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1991,7 +2063,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
@@ -2004,7 +2076,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -2017,7 +2089,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
@@ -2030,8 +2102,10 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="22" t="s">
+        <v>238</v>
+      </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2">
@@ -2041,8 +2115,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="22" t="s">
+        <v>239</v>
+      </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2">
@@ -2052,8 +2128,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="22" t="s">
+        <v>240</v>
+      </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2">
@@ -2063,8 +2141,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="22" t="s">
+        <v>241</v>
+      </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
@@ -2074,8 +2154,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="22" t="s">
+        <v>242</v>
+      </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2">
@@ -2085,8 +2167,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="23" t="s">
+        <v>243</v>
+      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2">
@@ -2096,8 +2180,10 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="22" t="s">
+        <v>244</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2">
@@ -2107,8 +2193,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="22" t="s">
+        <v>245</v>
+      </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2">
@@ -2118,8 +2206,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="23" t="s">
+        <v>246</v>
+      </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2">
@@ -2129,8 +2219,10 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="23" t="s">
+        <v>247</v>
+      </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2">
@@ -2140,8 +2232,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="22" t="s">
+        <v>248</v>
+      </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2">
@@ -2151,7 +2245,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2162,7 +2256,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2173,7 +2267,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2184,7 +2278,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2195,7 +2289,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2206,7 +2300,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2217,7 +2311,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2228,7 +2322,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2239,7 +2333,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2250,7 +2344,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2261,7 +2355,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2272,7 +2366,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2283,7 +2377,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2294,7 +2388,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2305,7 +2399,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2316,7 +2410,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2327,7 +2421,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2338,7 +2432,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2349,7 +2443,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2360,7 +2454,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2371,7 +2465,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2382,7 +2476,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2393,7 +2487,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2404,7 +2498,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2415,7 +2509,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2426,7 +2520,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2437,7 +2531,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2448,7 +2542,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2459,7 +2553,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2470,7 +2564,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2481,7 +2575,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2492,7 +2586,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2503,7 +2597,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2514,7 +2608,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2525,7 +2619,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2536,7 +2630,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2547,7 +2641,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2558,7 +2652,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2569,7 +2663,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2580,7 +2674,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2591,7 +2685,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2602,7 +2696,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2613,7 +2707,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2624,7 +2718,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2635,7 +2729,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2646,7 +2740,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2657,7 +2751,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2668,7 +2762,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2679,7 +2773,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2690,7 +2784,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2701,7 +2795,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2712,7 +2806,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2723,7 +2817,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2734,7 +2828,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2745,7 +2839,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2756,7 +2850,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2767,7 +2861,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2778,7 +2872,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2789,7 +2883,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2800,7 +2894,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2811,7 +2905,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2822,7 +2916,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2833,7 +2927,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2844,7 +2938,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2855,7 +2949,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2866,7 +2960,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2877,7 +2971,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2888,7 +2982,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2899,7 +2993,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2910,7 +3004,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -2921,7 +3015,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -2932,7 +3026,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -2943,7 +3037,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -2954,7 +3048,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -2965,7 +3059,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -2976,7 +3070,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -2987,7 +3081,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -2998,7 +3092,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3009,7 +3103,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3020,7 +3114,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3031,7 +3125,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3042,7 +3136,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3053,7 +3147,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3064,7 +3158,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3075,7 +3169,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3086,7 +3180,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3097,7 +3191,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3108,7 +3202,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3119,7 +3213,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3130,7 +3224,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3141,7 +3235,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3152,7 +3246,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3163,7 +3257,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3174,7 +3268,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3185,7 +3279,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3196,7 +3290,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3207,7 +3301,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3218,7 +3312,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3229,7 +3323,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3240,7 +3334,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3251,7 +3345,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3262,7 +3356,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3273,7 +3367,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3284,7 +3378,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3295,7 +3389,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3306,7 +3400,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3317,7 +3411,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3328,7 +3422,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3339,7 +3433,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3350,7 +3444,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3361,7 +3455,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3372,7 +3466,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3383,7 +3477,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3394,7 +3488,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3405,7 +3499,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3416,7 +3510,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3427,7 +3521,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3438,7 +3532,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3449,7 +3543,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3460,7 +3554,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3471,7 +3565,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3482,7 +3576,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3493,7 +3587,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3504,7 +3598,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3515,7 +3609,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3526,7 +3620,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3537,7 +3631,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3548,7 +3642,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3559,7 +3653,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3570,7 +3664,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3581,7 +3675,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3592,7 +3686,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3603,7 +3697,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3614,7 +3708,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="2"/>
@@ -3625,11 +3719,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C186" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6ZM3hTAdwDPMQ24jf/kwcZor1AjZ3jzLTNh2NSWTskM5eOzhWM/AiGX10pNn5MBtVdULyKtdwlUDBz0H0UwEew==" saltValue="erjZh30KLhrkeXUDQrmtYQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G186">
     <sortCondition ref="G1:G186"/>
   </sortState>

</xml_diff>

<commit_message>
AC-185. Bulk upload template changes
Modified template to accept data in row-wise order
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE9639D-E76A-4A8B-9FE4-03B465304A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="alxn1tfLV0ACcanmzFzwTVyJPnlpuZNJyyx/rb/FszFdv1B5BeHBqJka/kM6jlPW4d7Q7v6cagY7razCe35cHw==" workbookSaltValue="fE0BMcmvM7rJbjYqd46DsA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31A0A39-9603-4E3C-BD5F-ACBFF0F84CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="veryHidden" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -798,8 +797,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -824,7 +824,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -834,12 +834,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -989,35 +983,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1334,143 +1330,306 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AF4C19-D9D8-4D17-BA71-C91E169BA22D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="11"/>
+    <col min="1" max="1" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="H1" s="14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="I1" s="14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="J1" s="14" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="K1" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="L1" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+    </row>
+    <row r="3" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="5" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+    </row>
+    <row r="12" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+    </row>
+    <row r="13" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tACaLL4t6D1qLp0aJW8R+Wabszhwe0yefTNPvDvU/qRivSan/MPr1o7MgITTPt/8RcYCMHNmNbfFpzI/Qhq+Ow==" saltValue="LZJn8RIEcbMgbutCtlxKDA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:XFD1" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
+  <sheetProtection algorithmName="SHA-512" hashValue="ZBQLyGvaJPrMPSDPmjzbmqAk8bXnx3WUiQcZkFmojSC52JsC+HSZI9WSr8BgcSNOyIjR3ZnoUmMvJEcDjOydSw==" saltValue="SdaL5pEHj9MA0GpJvN41SA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
+  <dataValidations count="6">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:L1 A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:XFD7" xr:uid="{E26CAB39-A4D5-4CDD-A869-59535BC6FDF5}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 B2:B1048576" xr:uid="{820604F4-ED75-4A4C-AC98-FF2036A48C8C}">
+      <formula1>40909</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 F2:F1048576" xr:uid="{01C54EDB-8CDE-4226-AD78-37C83EDB08F0}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1" xr:uid="{E26CAB39-A4D5-4CDD-A869-59535BC6FDF5}">
       <formula1>-99999999999999</formula1>
       <formula2>99999999999999</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:XFD10" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:XFD2" xr:uid="{820604F4-ED75-4A4C-AC98-FF2036A48C8C}">
-      <formula1>40909</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:XFD6" xr:uid="{01C54EDB-8CDE-4226-AD78-37C83EDB08F0}">
-      <formula1>0</formula1>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{E533A554-9CC9-47C2-BDCE-4B2C5D519B1A}">
+      <formula1>-99999999999</formula1>
+      <formula2>99999999999</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{270CF3BB-5B9B-40EC-8A02-7CFFCB3B95C5}">
           <x14:formula1>
             <xm:f>Sheet2!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:XFD7 XEF4:XFD4 B4:XEE4</xm:sqref>
+          <xm:sqref>H1 K1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
+          <x14:formula1>
+            <xm:f>Sheet2!$C$1:$C$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5921C6A4-2CD9-4EAE-9809-BA84C4675AA1}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$52</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:XFD3</xm:sqref>
+          <xm:sqref>G1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85863E50-D527-4AC5-A2D8-C6D4BC7E5ACE}">
+          <x14:formula1>
+            <xm:f>Sheet2!$I$1:$I$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>I1 E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD33D8DB-60D7-4F0B-971A-5F8F33CA4B56}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B8:XFD8</xm:sqref>
+          <xm:sqref>L1 H2:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CA0AD2C-0AF4-4BD4-9B65-21E28E153E4A}">
+        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BB1558C-DA49-446D-8D32-92277B04523E}">
           <x14:formula1>
-            <xm:f>Sheet2!$H$1:$H$2</xm:f>
+            <xm:f>Sheet2!$A$4:$A$52</xm:f>
           </x14:formula1>
-          <xm:sqref>B13:XFD13</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00ECCC13-F8BB-4BC7-9E76-CE6657AC06A8}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$18</xm:f>
+            <xm:f>Sheet2!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B9:XFD9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85863E50-D527-4AC5-A2D8-C6D4BC7E5ACE}">
-          <x14:formula1>
-            <xm:f>Sheet2!$I$1:$I$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5:XFD5</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1483,18 +1642,18 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I186"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="21"/>
+    <col min="1" max="1" width="16.21875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1513,11 +1672,11 @@
       <c r="E1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="12" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="10" t="s">
         <v>231</v>
       </c>
     </row>
@@ -1537,11 +1696,11 @@
       <c r="E2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="10" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1561,10 +1720,10 @@
       <c r="E3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>232</v>
       </c>
     </row>
@@ -1584,10 +1743,10 @@
       <c r="E4" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>233</v>
       </c>
     </row>
@@ -1607,10 +1766,10 @@
       <c r="E5" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="10" t="s">
         <v>208</v>
       </c>
     </row>
@@ -1628,7 +1787,7 @@
       <c r="E6" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="10" t="s">
         <v>209</v>
       </c>
     </row>
@@ -1646,7 +1805,7 @@
       <c r="E7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="10" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1664,7 +1823,7 @@
       <c r="E8" s="6">
         <v>871668</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="10" t="s">
         <v>234</v>
       </c>
     </row>
@@ -1682,7 +1841,7 @@
       <c r="E9" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>235</v>
       </c>
     </row>
@@ -1700,7 +1859,7 @@
       <c r="E10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="10" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2111,7 +2270,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="18" t="s">
         <v>238</v>
       </c>
       <c r="B41" s="2"/>
@@ -2124,7 +2283,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="18" t="s">
         <v>239</v>
       </c>
       <c r="B42" s="2"/>
@@ -2137,7 +2296,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="18" t="s">
         <v>240</v>
       </c>
       <c r="B43" s="2"/>
@@ -2150,7 +2309,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="18" t="s">
         <v>241</v>
       </c>
       <c r="B44" s="2"/>
@@ -2163,7 +2322,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="18" t="s">
         <v>242</v>
       </c>
       <c r="B45" s="2"/>
@@ -2176,7 +2335,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="19" t="s">
         <v>243</v>
       </c>
       <c r="B46" s="2"/>
@@ -2189,7 +2348,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="18" t="s">
         <v>244</v>
       </c>
       <c r="B47" s="2"/>
@@ -2202,7 +2361,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="18" t="s">
         <v>245</v>
       </c>
       <c r="B48" s="2"/>
@@ -2215,7 +2374,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="19" t="s">
         <v>246</v>
       </c>
       <c r="B49" s="2"/>
@@ -2228,7 +2387,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="19" t="s">
         <v>247</v>
       </c>
       <c r="B50" s="2"/>
@@ -2241,7 +2400,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="18" t="s">
         <v>248</v>
       </c>
       <c r="B51" s="2"/>

</xml_diff>

<commit_message>
AC-203. Bulk upload template subtype addition, amount field name change.
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31A0A39-9603-4E3C-BD5F-ACBFF0F84CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27229AC2-4649-4E2F-8B71-11512EE9E8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="QffQiebz39Y+uvLYV2A0QeNuAsxxzjbHwfy6Zjp6cIlGFqntCImu13njeKg2FyTBxEbMLD0QSf8ru7X7pWZU1g==" workbookSaltValue="QsSowoUqKR5FQKk/s3jLnQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="253">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -712,9 +713,6 @@
     <t>Call Date</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>Wso Asset ID</t>
   </si>
   <si>
@@ -791,6 +789,12 @@
   </si>
   <si>
     <t>Over/Under call on Investments</t>
+  </si>
+  <si>
+    <t>Equalization interest expenses</t>
+  </si>
+  <si>
+    <t>Amount (in Fund Ccy)</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1349,7 @@
     <col min="4" max="4" width="12.5546875" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="23" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" style="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="22" bestFit="1" customWidth="1"/>
@@ -1368,13 +1372,13 @@
         <v>207</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>228</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>1</v>
@@ -1383,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>48</v>
@@ -1561,23 +1565,19 @@
       <c r="L13" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ZBQLyGvaJPrMPSDPmjzbmqAk8bXnx3WUiQcZkFmojSC52JsC+HSZI9WSr8BgcSNOyIjR3ZnoUmMvJEcDjOydSw==" saltValue="SdaL5pEHj9MA0GpJvN41SA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
-  <dataValidations count="6">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:L1 A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
+  <sheetProtection algorithmName="SHA-512" hashValue="ejfXfmjFBm4fAFFZbf5OzNoQDDmWIkdv+0BusjV2bsZdO9T/3ikPpIbL+mmd0LbsTBuWHWaaDGajn6tkKoKq0Q==" saltValue="mLUBkiG5IPRQ2ch+HJC+mw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
+  <dataValidations count="5">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 B2:B1048576" xr:uid="{820604F4-ED75-4A4C-AC98-FF2036A48C8C}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{820604F4-ED75-4A4C-AC98-FF2036A48C8C}">
       <formula1>40909</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 F2:F1048576" xr:uid="{01C54EDB-8CDE-4226-AD78-37C83EDB08F0}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{01C54EDB-8CDE-4226-AD78-37C83EDB08F0}">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1" xr:uid="{E26CAB39-A4D5-4CDD-A869-59535BC6FDF5}">
-      <formula1>-99999999999999</formula1>
-      <formula2>99999999999999</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{E533A554-9CC9-47C2-BDCE-4B2C5D519B1A}">
       <formula1>-99999999999</formula1>
@@ -1588,36 +1588,24 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{270CF3BB-5B9B-40EC-8A02-7CFFCB3B95C5}">
-          <x14:formula1>
-            <xm:f>Sheet2!$G$1:$G$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>H1 K1</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$18</xm:f>
+            <xm:f>Sheet2!$C$1:$C$19</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5921C6A4-2CD9-4EAE-9809-BA84C4675AA1}">
-          <x14:formula1>
-            <xm:f>Sheet2!$A$1:$A$52</xm:f>
-          </x14:formula1>
-          <xm:sqref>G1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85863E50-D527-4AC5-A2D8-C6D4BC7E5ACE}">
           <x14:formula1>
             <xm:f>Sheet2!$I$1:$I$10</xm:f>
           </x14:formula1>
-          <xm:sqref>I1 E2:E1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD33D8DB-60D7-4F0B-971A-5F8F33CA4B56}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>L1 H2:H1048576</xm:sqref>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BB1558C-DA49-446D-8D32-92277B04523E}">
           <x14:formula1>
@@ -1643,7 +1631,7 @@
   <dimension ref="A1:I186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,7 +1665,7 @@
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1724,7 +1712,7 @@
         <v>209</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1747,7 +1735,7 @@
         <v>212</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1824,7 +1812,7 @@
         <v>871668</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1833,7 +1821,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D9" s="2">
         <v>74</v>
@@ -1842,7 +1830,7 @@
         <v>86</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1914,7 +1902,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D14" s="2">
         <v>129</v>
@@ -1929,7 +1917,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D15" s="2">
         <v>130</v>
@@ -1944,7 +1932,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D16" s="2">
         <v>141</v>
@@ -1959,7 +1947,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D17" s="2">
         <v>142</v>
@@ -1974,7 +1962,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D18" s="2">
         <v>148</v>
@@ -1988,7 +1976,9 @@
         <v>21</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>251</v>
+      </c>
       <c r="D19" s="2">
         <v>158</v>
       </c>
@@ -2271,7 +2261,7 @@
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2284,7 +2274,7 @@
     </row>
     <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2297,7 +2287,7 @@
     </row>
     <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2310,7 +2300,7 @@
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2323,7 +2313,7 @@
     </row>
     <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2336,7 +2326,7 @@
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2349,7 +2339,7 @@
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2362,7 +2352,7 @@
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2375,7 +2365,7 @@
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2388,7 +2378,7 @@
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2401,7 +2391,7 @@
     </row>
     <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2414,7 +2404,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>

</xml_diff>

<commit_message>
AC-203. Bulk upload template changes.
Changed access control table to mat-table
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27229AC2-4649-4E2F-8B71-11512EE9E8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640D1507-B399-42B0-A250-B4149745FC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="QffQiebz39Y+uvLYV2A0QeNuAsxxzjbHwfy6Zjp6cIlGFqntCImu13njeKg2FyTBxEbMLD0QSf8ru7X7pWZU1g==" workbookSaltValue="QsSowoUqKR5FQKk/s3jLnQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -1341,24 +1341,24 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" style="23" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.77734375" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="21"/>
+    <col min="7" max="7" width="19.42578125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="22"/>
@@ -1410,7 +1410,7 @@
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="22"/>
@@ -1424,7 +1424,7 @@
       <c r="K3" s="22"/>
       <c r="L3" s="22"/>
     </row>
-    <row r="4" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="22"/>
@@ -1438,7 +1438,7 @@
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="22"/>
@@ -1452,7 +1452,7 @@
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
     </row>
-    <row r="6" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="22"/>
@@ -1466,7 +1466,7 @@
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
     </row>
-    <row r="7" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="22"/>
@@ -1480,7 +1480,7 @@
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
     </row>
-    <row r="8" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="22"/>
@@ -1494,7 +1494,7 @@
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
     </row>
-    <row r="9" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="22"/>
@@ -1508,7 +1508,7 @@
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
     </row>
-    <row r="10" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="22"/>
@@ -1522,7 +1522,7 @@
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
     </row>
-    <row r="11" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="22"/>
@@ -1536,7 +1536,7 @@
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
     </row>
-    <row r="12" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="22"/>
@@ -1550,7 +1550,7 @@
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
     </row>
-    <row r="13" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="22"/>
@@ -1565,7 +1565,7 @@
       <c r="L13" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ejfXfmjFBm4fAFFZbf5OzNoQDDmWIkdv+0BusjV2bsZdO9T/3ikPpIbL+mmd0LbsTBuWHWaaDGajn6tkKoKq0Q==" saltValue="mLUBkiG5IPRQ2ch+HJC+mw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="K+oJktqUe4PSbuJlWLVQZfC63mKwLL4p7BZYiBQw9wnXCPVVhvj3j1qMergT/KocQF6PeftU6kH6mvDl7TjO1A==" saltValue="Yg9MiyZy55c9xGP9cuUG1Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1634,17 +1634,17 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="17"/>
+    <col min="5" max="5" width="44.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>237</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
         <v>238</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
         <v>239</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
         <v>240</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
         <v>241</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>242</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
         <v>243</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
         <v>244</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="s">
         <v>245</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
         <v>246</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
         <v>247</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2426,7 +2426,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2437,7 +2437,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2448,7 +2448,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2459,7 +2459,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2470,7 +2470,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2481,7 +2481,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2492,7 +2492,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2503,7 +2503,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2514,7 +2514,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2525,7 +2525,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2536,7 +2536,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2547,7 +2547,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2558,7 +2558,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2569,7 +2569,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2580,7 +2580,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2591,7 +2591,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2602,7 +2602,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2613,7 +2613,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2624,7 +2624,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2635,7 +2635,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2646,7 +2646,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2657,7 +2657,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2668,7 +2668,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2679,7 +2679,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2690,7 +2690,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2701,7 +2701,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2712,7 +2712,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2723,7 +2723,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2734,7 +2734,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2745,7 +2745,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2756,7 +2756,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2767,7 +2767,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2778,7 +2778,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2789,7 +2789,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2800,7 +2800,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2811,7 +2811,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2822,7 +2822,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2833,7 +2833,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2844,7 +2844,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2855,7 +2855,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2866,7 +2866,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2877,7 +2877,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2888,7 +2888,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2899,7 +2899,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2910,7 +2910,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2921,7 +2921,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2932,7 +2932,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2943,7 +2943,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2954,7 +2954,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2965,7 +2965,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2976,7 +2976,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2987,7 +2987,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2998,7 +2998,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3009,7 +3009,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3020,7 +3020,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3031,7 +3031,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3042,7 +3042,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3053,7 +3053,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3064,7 +3064,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3075,7 +3075,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3086,7 +3086,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3097,7 +3097,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3108,7 +3108,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3119,7 +3119,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3130,7 +3130,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3141,7 +3141,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3152,7 +3152,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3163,7 +3163,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3174,7 +3174,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3185,7 +3185,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3196,7 +3196,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3207,7 +3207,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3218,7 +3218,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3229,7 +3229,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3240,7 +3240,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3251,7 +3251,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3262,7 +3262,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3273,7 +3273,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3284,7 +3284,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3295,7 +3295,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3306,7 +3306,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3317,7 +3317,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3328,7 +3328,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3339,7 +3339,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3350,7 +3350,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3361,7 +3361,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3372,7 +3372,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3383,7 +3383,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3394,7 +3394,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3405,7 +3405,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3416,7 +3416,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3427,7 +3427,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3438,7 +3438,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3449,7 +3449,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3460,7 +3460,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3471,7 +3471,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3482,7 +3482,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3493,7 +3493,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3504,7 +3504,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3515,7 +3515,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3526,7 +3526,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3537,7 +3537,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3548,7 +3548,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3559,7 +3559,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3570,7 +3570,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3581,7 +3581,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3592,7 +3592,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3603,7 +3603,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3614,7 +3614,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3625,7 +3625,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3636,7 +3636,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3647,7 +3647,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3658,7 +3658,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3669,7 +3669,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3680,7 +3680,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3691,7 +3691,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3702,7 +3702,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3713,7 +3713,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3724,7 +3724,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3735,7 +3735,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3746,7 +3746,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3757,7 +3757,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3768,7 +3768,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3779,7 +3779,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3790,7 +3790,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3801,7 +3801,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3812,7 +3812,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3823,7 +3823,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3834,7 +3834,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3845,7 +3845,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3856,7 +3856,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3867,7 +3867,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="2"/>
@@ -3878,7 +3878,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C186" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AC-205. GIR Feed from Capital Activity to AssetGIR
Added GIR Override column in bulk upload template.
Added GIR Override checkbox in single add/edit capital activity.
Added GIR Source id, source columns on CA grid.
Added IsOverride, SourceID, Source columns on GIR Editor screen to view.
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,8 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640D1507-B399-42B0-A250-B4149745FC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="QffQiebz39Y+uvLYV2A0QeNuAsxxzjbHwfy6Zjp6cIlGFqntCImu13njeKg2FyTBxEbMLD0QSf8ru7X7pWZU1g==" workbookSaltValue="QsSowoUqKR5FQKk/s3jLnQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29224849-038E-463E-BCBA-C031549F490F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="6K/Q7F124n2WA74ChF5MoCQQLTCFkER0D8N+zyeqg98+Q/WaMeGzoi7X0rCRvHMdamaXBQWkx6v21yKWKvktPA==" workbookSaltValue="WBnEwnKq7LB4UTCsDTFpOw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="256">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -795,6 +795,15 @@
   </si>
   <si>
     <t>Amount (in Fund Ccy)</t>
+  </si>
+  <si>
+    <t>GIR Override</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1343,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AF4C19-D9D8-4D17-BA71-C91E169BA22D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1349,16 +1358,17 @@
     <col min="4" max="4" width="12.5703125" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="21"/>
+    <col min="7" max="7" width="17" style="22" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="23" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1378,199 +1388,214 @@
         <v>227</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
-    </row>
-    <row r="3" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
       <c r="L3" s="22"/>
-    </row>
-    <row r="4" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
-    </row>
-    <row r="5" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="22"/>
+    </row>
+    <row r="5" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
-    </row>
-    <row r="6" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="22"/>
+    </row>
+    <row r="6" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
-    </row>
-    <row r="7" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="22"/>
+    </row>
+    <row r="7" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
-    </row>
-    <row r="8" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="22"/>
+    </row>
+    <row r="8" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="22"/>
+    </row>
+    <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="22"/>
+    </row>
+    <row r="10" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
-    </row>
-    <row r="11" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="22"/>
+    </row>
+    <row r="11" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
-    </row>
-    <row r="12" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="22"/>
+    </row>
+    <row r="12" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
-    </row>
-    <row r="13" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="22"/>
+    </row>
+    <row r="13" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="K+oJktqUe4PSbuJlWLVQZfC63mKwLL4p7BZYiBQw9wnXCPVVhvj3j1qMergT/KocQF6PeftU6kH6mvDl7TjO1A==" saltValue="Yg9MiyZy55c9xGP9cuUG1Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hU2JMp2RN+qd+SOJ7ll9lI5tQidbWQUIJkr9hhSoIiUfAzhaLbueSSI5OB/CwyEYWm0bSRs0PtcbGL3M//3ZdA==" saltValue="+Xlcef2lhuDXkQq7wTkPPg==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{820604F4-ED75-4A4C-AC98-FF2036A48C8C}">
@@ -1579,7 +1604,7 @@
     <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{01C54EDB-8CDE-4226-AD78-37C83EDB08F0}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{E533A554-9CC9-47C2-BDCE-4B2C5D519B1A}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{E533A554-9CC9-47C2-BDCE-4B2C5D519B1A}">
       <formula1>-99999999999</formula1>
       <formula2>99999999999</formula2>
     </dataValidation>
@@ -1588,12 +1613,12 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
           <x14:formula1>
             <xm:f>Sheet2!$C$1:$C$19</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85863E50-D527-4AC5-A2D8-C6D4BC7E5ACE}">
           <x14:formula1>
@@ -1605,7 +1630,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BB1558C-DA49-446D-8D32-92277B04523E}">
           <x14:formula1>
@@ -1619,6 +1644,12 @@
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FF313E70-3069-4053-8087-E42997D2EC86}">
+          <x14:formula1>
+            <xm:f>Sheet2!$J$1:$J$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1 G2:G1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1628,10 +1659,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE38E7C1-F75A-461B-83D8-D3E941B09876}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:J186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,7 +1675,7 @@
     <col min="6" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1667,8 +1698,11 @@
       <c r="I1" s="10" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1691,8 +1725,11 @@
       <c r="I2" s="10" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1715,7 +1752,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1738,7 +1775,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1761,7 +1798,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1779,7 +1816,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1797,7 +1834,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1815,7 +1852,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1833,7 +1870,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1851,7 +1888,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1866,7 +1903,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1881,7 +1918,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1896,7 +1933,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1911,7 +1948,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1926,7 +1963,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Updating git HEAD to previous commit 635fd54
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skumar\source\ArkRepo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6369082A-46DF-4A52-9847-4EB9EF73E342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29224849-038E-463E-BCBA-C031549F490F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="6K/Q7F124n2WA74ChF5MoCQQLTCFkER0D8N+zyeqg98+Q/WaMeGzoi7X0rCRvHMdamaXBQWkx6v21yKWKvktPA==" workbookSaltValue="WBnEwnKq7LB4UTCsDTFpOw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="256">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -712,9 +713,6 @@
     <t>Call Date</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
     <t>Wso Asset ID</t>
   </si>
   <si>
@@ -743,16 +741,80 @@
   </si>
   <si>
     <t xml:space="preserve">SEK </t>
+  </si>
+  <si>
+    <t>Advanced Tax Distribution</t>
+  </si>
+  <si>
+    <t>Carry</t>
+  </si>
+  <si>
+    <t>DL410EUR</t>
+  </si>
+  <si>
+    <t>DL47EUR</t>
+  </si>
+  <si>
+    <t>DL47GBP</t>
+  </si>
+  <si>
+    <t>DL47JPY</t>
+  </si>
+  <si>
+    <t>DL47USD</t>
+  </si>
+  <si>
+    <t>DL4LEV10EUR</t>
+  </si>
+  <si>
+    <t>DL4LEV7EUR</t>
+  </si>
+  <si>
+    <t>DL4LEV7USD</t>
+  </si>
+  <si>
+    <t>DL4LEVS7EUR</t>
+  </si>
+  <si>
+    <t>DL4LEVS7USD</t>
+  </si>
+  <si>
+    <t>DL4S10EUR</t>
+  </si>
+  <si>
+    <t>GIR Cash Adj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DL4S7EUR </t>
+  </si>
+  <si>
+    <t>Over/Under call on Investments</t>
+  </si>
+  <si>
+    <t>Equalization interest expenses</t>
+  </si>
+  <si>
+    <t>Amount (in Fund Ccy)</t>
+  </si>
+  <si>
+    <t>GIR Override</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,6 +825,13 @@
     <font>
       <sz val="11"/>
       <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -783,18 +852,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor rgb="FFAEAAAA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -897,11 +966,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -912,30 +996,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,101 +1343,270 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AF4C19-D9D8-4D17-BA71-C91E169BA22D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="22" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="23" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="E1" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="G1" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="L1" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="M1" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+    </row>
+    <row r="5" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+    </row>
+    <row r="6" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+    </row>
+    <row r="7" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+    </row>
+    <row r="8" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+    </row>
+    <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+    </row>
+    <row r="10" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+    </row>
+    <row r="11" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+    </row>
+    <row r="12" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+    </row>
+    <row r="13" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XqeHUEzh+dyHP9uUApM1BZusiPZVmm7iLwiYSuPqCgvL6a176n3EBzSW8w8Fw9znuR6gXJtJHdSOm6UA4w26BQ==" saltValue="Jnk2HtyEQHMKBBcNB3BZPw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hU2JMp2RN+qd+SOJ7ll9lI5tQidbWQUIJkr9hhSoIiUfAzhaLbueSSI5OB/CwyEYWm0bSRs0PtcbGL3M//3ZdA==" saltValue="+Xlcef2lhuDXkQq7wTkPPg==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="5">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:XFD1" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:XFD7" xr:uid="{E26CAB39-A4D5-4CDD-A869-59535BC6FDF5}">
-      <formula1>-99999999999999</formula1>
-      <formula2>99999999999999</formula2>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:XFD10" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{47360A1B-DA98-4424-9A3D-70A12D0701E9}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:XFD2" xr:uid="{820604F4-ED75-4A4C-AC98-FF2036A48C8C}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{820604F4-ED75-4A4C-AC98-FF2036A48C8C}">
       <formula1>40909</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:XFD6" xr:uid="{01C54EDB-8CDE-4226-AD78-37C83EDB08F0}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{01C54EDB-8CDE-4226-AD78-37C83EDB08F0}">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{E533A554-9CC9-47C2-BDCE-4B2C5D519B1A}">
+      <formula1>-99999999999</formula1>
+      <formula2>99999999999</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1353,41 +1614,41 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{270CF3BB-5B9B-40EC-8A02-7CFFCB3B95C5}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
           <x14:formula1>
-            <xm:f>Sheet2!$G$1:$G$5</xm:f>
+            <xm:f>Sheet2!$C$1:$C$19</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:XFD7 XEF4:XFD4 B4:XEE4</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5921C6A4-2CD9-4EAE-9809-BA84C4675AA1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85863E50-D527-4AC5-A2D8-C6D4BC7E5ACE}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$1:$A$40</xm:f>
+            <xm:f>Sheet2!$I$1:$I$10</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:XFD3</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD33D8DB-60D7-4F0B-971A-5F8F33CA4B56}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B8:XFD8</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CA0AD2C-0AF4-4BD4-9B65-21E28E153E4A}">
+        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BB1558C-DA49-446D-8D32-92277B04523E}">
           <x14:formula1>
-            <xm:f>Sheet2!$H$1:$H$2</xm:f>
+            <xm:f>Sheet2!$A$4:$A$52</xm:f>
           </x14:formula1>
-          <xm:sqref>B13:XFD13</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00ECCC13-F8BB-4BC7-9E76-CE6657AC06A8}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$14</xm:f>
+            <xm:f>Sheet2!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B9:XFD9</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85863E50-D527-4AC5-A2D8-C6D4BC7E5ACE}">
+        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FF313E70-3069-4053-8087-E42997D2EC86}">
           <x14:formula1>
-            <xm:f>Sheet2!$I$1:$I$10</xm:f>
+            <xm:f>Sheet2!$J$1:$J$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:XFD5</xm:sqref>
+          <xm:sqref>G1 G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1398,23 +1659,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE38E7C1-F75A-461B-83D8-D3E941B09876}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:J186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="16.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1430,15 +1691,18 @@
       <c r="E1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="16"/>
+      <c r="I1" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1454,15 +1718,18 @@
       <c r="E2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="10" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1478,14 +1745,14 @@
       <c r="E3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1501,14 +1768,14 @@
       <c r="E4" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1524,14 +1791,14 @@
       <c r="E5" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="10" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1545,11 +1812,11 @@
       <c r="E6" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="10" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1563,11 +1830,11 @@
       <c r="E7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="10" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1581,17 +1848,17 @@
       <c r="E8" s="6">
         <v>871668</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D9" s="2">
         <v>74</v>
@@ -1599,11 +1866,11 @@
       <c r="E9" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1617,11 +1884,11 @@
       <c r="E10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="10" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1636,7 +1903,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1651,7 +1918,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1666,13 +1933,13 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D14" s="2">
         <v>129</v>
@@ -1681,12 +1948,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>235</v>
+      </c>
       <c r="D15" s="2">
         <v>130</v>
       </c>
@@ -1694,12 +1963,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="D16" s="2">
         <v>141</v>
       </c>
@@ -1707,12 +1978,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>248</v>
+      </c>
       <c r="D17" s="2">
         <v>142</v>
       </c>
@@ -1720,12 +1993,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" t="s">
+        <v>250</v>
+      </c>
       <c r="D18" s="2">
         <v>148</v>
       </c>
@@ -1733,12 +2008,14 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>251</v>
+      </c>
       <c r="D19" s="2">
         <v>158</v>
       </c>
@@ -1746,7 +2023,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1759,7 +2036,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -1772,7 +2049,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -1785,7 +2062,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -1798,7 +2075,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -1811,7 +2088,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -1824,7 +2101,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -1837,7 +2114,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
@@ -1850,7 +2127,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -1863,7 +2140,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
@@ -1876,7 +2153,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
@@ -1889,7 +2166,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
@@ -1902,7 +2179,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
@@ -1915,7 +2192,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -1928,7 +2205,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -1941,7 +2218,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
@@ -1954,7 +2231,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
@@ -1967,7 +2244,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1980,7 +2257,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
@@ -1993,7 +2270,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -2006,7 +2283,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
@@ -2019,8 +2296,10 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>237</v>
+      </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2">
@@ -2030,8 +2309,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>238</v>
+      </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2">
@@ -2041,8 +2322,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
+        <v>239</v>
+      </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2">
@@ -2052,8 +2335,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>240</v>
+      </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
@@ -2063,8 +2348,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
+        <v>241</v>
+      </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2">
@@ -2074,8 +2361,10 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>242</v>
+      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2">
@@ -2085,8 +2374,10 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18" t="s">
+        <v>243</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2">
@@ -2096,8 +2387,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18" t="s">
+        <v>244</v>
+      </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2">
@@ -2107,8 +2400,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="19" t="s">
+        <v>245</v>
+      </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2">
@@ -2118,8 +2413,10 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="19" t="s">
+        <v>246</v>
+      </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2">
@@ -2129,8 +2426,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
+    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
+        <v>247</v>
+      </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2">
@@ -2140,8 +2439,10 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>249</v>
+      </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2">
@@ -2151,7 +2452,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2162,7 +2463,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2173,7 +2474,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2184,7 +2485,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2195,7 +2496,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2206,7 +2507,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2217,7 +2518,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2228,7 +2529,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2239,7 +2540,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2250,7 +2551,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2261,7 +2562,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2272,7 +2573,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2283,7 +2584,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2294,7 +2595,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2305,7 +2606,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2316,7 +2617,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2327,7 +2628,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2338,7 +2639,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2349,7 +2650,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2360,7 +2661,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2371,7 +2672,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2382,7 +2683,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2393,7 +2694,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2404,7 +2705,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2415,7 +2716,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2426,7 +2727,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2437,7 +2738,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2448,7 +2749,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2459,7 +2760,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2470,7 +2771,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2481,7 +2782,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2492,7 +2793,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2503,7 +2804,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2514,7 +2815,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2525,7 +2826,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2536,7 +2837,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2547,7 +2848,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2558,7 +2859,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2569,7 +2870,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2580,7 +2881,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2591,7 +2892,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2602,7 +2903,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2613,7 +2914,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2624,7 +2925,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2635,7 +2936,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2646,7 +2947,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2657,7 +2958,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2668,7 +2969,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2679,7 +2980,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2690,7 +2991,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2701,7 +3002,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2712,7 +3013,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2723,7 +3024,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2734,7 +3035,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2745,7 +3046,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2756,7 +3057,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2767,7 +3068,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2778,7 +3079,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2789,7 +3090,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2800,7 +3101,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2811,7 +3112,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="113" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2822,7 +3123,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2833,7 +3134,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2844,7 +3145,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2855,7 +3156,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -2866,7 +3167,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="118" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -2877,7 +3178,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="119" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -2888,7 +3189,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="120" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -2899,7 +3200,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -2910,7 +3211,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -2921,7 +3222,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -2932,7 +3233,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -2943,7 +3244,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -2954,7 +3255,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -2965,7 +3266,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -2976,7 +3277,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -2987,7 +3288,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -2998,7 +3299,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3009,7 +3310,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3020,7 +3321,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3031,7 +3332,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3042,7 +3343,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3053,7 +3354,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3064,7 +3365,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3075,7 +3376,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3086,7 +3387,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3097,7 +3398,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3108,7 +3409,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3119,7 +3420,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="141" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3130,7 +3431,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3141,7 +3442,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3152,7 +3453,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3163,7 +3464,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3174,7 +3475,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3185,7 +3486,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3196,7 +3497,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3207,7 +3508,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3218,7 +3519,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3229,7 +3530,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="151" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3240,7 +3541,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3251,7 +3552,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3262,7 +3563,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3273,7 +3574,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3284,7 +3585,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3295,7 +3596,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3306,7 +3607,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3317,7 +3618,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="159" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3328,7 +3629,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3339,7 +3640,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3350,7 +3651,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3361,7 +3662,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3372,7 +3673,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3383,7 +3684,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3394,7 +3695,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3405,7 +3706,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3416,7 +3717,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3427,7 +3728,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3438,7 +3739,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3449,7 +3750,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="171" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3460,7 +3761,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3471,7 +3772,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3482,7 +3783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3493,7 +3794,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="175" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3504,7 +3805,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3515,7 +3816,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="177" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3526,7 +3827,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="178" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3537,7 +3838,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3548,7 +3849,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3559,7 +3860,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="181" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3570,7 +3871,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3581,7 +3882,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="183" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3592,7 +3893,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3603,7 +3904,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="185" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="2"/>
@@ -3614,11 +3915,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="186" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C186" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ANTEf2y0LtCbUqohELCtjXr4pdZNUHzyfZfxX48GZLeMwHLRkS5OWe4nvJ6cfomoaMi90pHAxUvbIxNzE4xzqA==" saltValue="hq7p2jAMvF47ZpAcRDQe0g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G186">
     <sortCondition ref="G1:G186"/>
   </sortState>

</xml_diff>

<commit_message>
Merged PR 49: Added SMA PRI, SMA HAIL HSBC, SMA GENERALI, SMA G2 fundhedgings to excel template
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,13 +5,13 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbharambe\Documents\Nisarg\Repo\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpol\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29224849-038E-463E-BCBA-C031549F490F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="6K/Q7F124n2WA74ChF5MoCQQLTCFkER0D8N+zyeqg98+Q/WaMeGzoi7X0rCRvHMdamaXBQWkx6v21yKWKvktPA==" workbookSaltValue="WBnEwnKq7LB4UTCsDTFpOw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130AEB6C-97A3-41CB-B938-6B6B40A84036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kC8cM+8NKgfNlXVeoq5zl6JRNnNR9PO0G60Jdw7TqaTbfLSEZ9nK8EFdniUSnnBb1qczKmXNKtSwprRxwcyB+A==" workbookSaltValue="zEbgma0RL1csL60XTK2z4w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="260">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -804,6 +804,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>SMA G2</t>
+  </si>
+  <si>
+    <t>SMA GENERALI</t>
+  </si>
+  <si>
+    <t>SMA PRI</t>
+  </si>
+  <si>
+    <t>SMA HAIL HSBC</t>
   </si>
 </sst>
 </file>
@@ -1347,28 +1359,28 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="22" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="23" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="21"/>
+    <col min="8" max="8" width="19.44140625" style="23" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1409,7 +1421,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="22"/>
@@ -1424,7 +1436,7 @@
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
     </row>
-    <row r="3" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="22"/>
@@ -1439,7 +1451,7 @@
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
     </row>
-    <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="22"/>
@@ -1454,7 +1466,7 @@
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
     </row>
-    <row r="5" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="22"/>
@@ -1469,7 +1481,7 @@
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
     </row>
-    <row r="6" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="22"/>
@@ -1484,7 +1496,7 @@
       <c r="L6" s="22"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="22"/>
@@ -1499,7 +1511,7 @@
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
     </row>
-    <row r="8" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="22"/>
@@ -1514,7 +1526,7 @@
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
     </row>
-    <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="22"/>
@@ -1529,7 +1541,7 @@
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
     </row>
-    <row r="10" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="22"/>
@@ -1544,7 +1556,7 @@
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
     </row>
-    <row r="11" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="22"/>
@@ -1559,7 +1571,7 @@
       <c r="L11" s="22"/>
       <c r="M11" s="22"/>
     </row>
-    <row r="12" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="22"/>
@@ -1574,7 +1586,7 @@
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
     </row>
-    <row r="13" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="22"/>
@@ -1590,7 +1602,7 @@
       <c r="M13" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="hU2JMp2RN+qd+SOJ7ll9lI5tQidbWQUIJkr9hhSoIiUfAzhaLbueSSI5OB/CwyEYWm0bSRs0PtcbGL3M//3ZdA==" saltValue="+Xlcef2lhuDXkQq7wTkPPg==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3TB3pj9S0mk47Ql/h8d/p4vhDYOoLbG6vyzq/HY/4/08ku3fLQtKQeiK2aTRZt4jZdmX6a2/EM9TdwOYmGbvRA==" saltValue="E4Hx5yIm54bcuKuwmcoj2Q==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1613,7 +1625,7 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
           <x14:formula1>
             <xm:f>Sheet2!$C$1:$C$19</xm:f>
@@ -1634,9 +1646,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BB1558C-DA49-446D-8D32-92277B04523E}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$4:$A$52</xm:f>
+            <xm:f>Sheet2!$A$4:$A$56</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>C2:C5 C7:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00ECCC13-F8BB-4BC7-9E76-CE6657AC06A8}">
           <x14:formula1>
@@ -1650,6 +1662,12 @@
           </x14:formula1>
           <xm:sqref>G1 G2:G1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BB1976F-BBF5-4D73-BB5B-CEA6D4D39945}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$4:$A$56</xm:f>
+          </x14:formula1>
+          <xm:sqref>C6</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1661,21 +1679,23 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="17"/>
+    <col min="5" max="5" width="44.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="9.109375" style="17"/>
+    <col min="12" max="12" width="9.109375" style="17" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +1722,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1749,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1752,7 +1772,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1775,7 +1795,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1798,7 +1818,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1816,7 +1836,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1834,7 +1854,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1872,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1870,7 +1890,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1888,7 +1908,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1903,7 +1923,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1918,7 +1938,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1933,7 +1953,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1948,7 +1968,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1963,7 +1983,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1978,7 +1998,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -1993,7 +2013,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -2008,7 +2028,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -2023,7 +2043,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -2036,7 +2056,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -2049,7 +2069,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -2062,7 +2082,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
@@ -2075,7 +2095,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -2088,7 +2108,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
@@ -2101,7 +2121,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
@@ -2114,7 +2134,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
@@ -2127,7 +2147,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
@@ -2140,7 +2160,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
@@ -2153,7 +2173,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>32</v>
       </c>
@@ -2166,7 +2186,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>33</v>
       </c>
@@ -2179,7 +2199,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>34</v>
       </c>
@@ -2192,7 +2212,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>35</v>
       </c>
@@ -2205,7 +2225,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -2218,7 +2238,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>37</v>
       </c>
@@ -2231,7 +2251,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>38</v>
       </c>
@@ -2244,7 +2264,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -2257,7 +2277,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
@@ -2270,7 +2290,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
@@ -2283,7 +2303,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
@@ -2296,7 +2316,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
         <v>237</v>
       </c>
@@ -2309,7 +2329,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
         <v>238</v>
       </c>
@@ -2322,7 +2342,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
         <v>239</v>
       </c>
@@ -2335,7 +2355,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
         <v>240</v>
       </c>
@@ -2348,7 +2368,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18" t="s">
         <v>241</v>
       </c>
@@ -2361,7 +2381,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="19" t="s">
         <v>242</v>
       </c>
@@ -2374,7 +2394,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18" t="s">
         <v>243</v>
       </c>
@@ -2387,7 +2407,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18" t="s">
         <v>244</v>
       </c>
@@ -2400,7 +2420,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="19" t="s">
         <v>245</v>
       </c>
@@ -2413,7 +2433,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="19" t="s">
         <v>246</v>
       </c>
@@ -2426,7 +2446,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>247</v>
       </c>
@@ -2439,7 +2459,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -2452,8 +2472,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>256</v>
+      </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2">
@@ -2463,8 +2485,10 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>257</v>
+      </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
@@ -2474,8 +2498,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2">
@@ -2485,8 +2511,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>258</v>
+      </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2">
@@ -2496,7 +2524,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="5"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2507,7 +2535,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="5"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2518,7 +2546,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="5"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2529,7 +2557,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="5"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2540,7 +2568,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2551,7 +2579,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2562,7 +2590,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="5"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2573,7 +2601,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="5"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2584,7 +2612,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2595,7 +2623,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2606,7 +2634,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2617,7 +2645,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2628,7 +2656,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2639,7 +2667,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2650,7 +2678,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2661,7 +2689,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2672,7 +2700,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2683,7 +2711,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2694,7 +2722,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2705,7 +2733,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2716,7 +2744,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2727,7 +2755,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2738,7 +2766,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2749,7 +2777,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2760,7 +2788,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2771,7 +2799,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2782,7 +2810,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2793,7 +2821,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2804,7 +2832,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2815,7 +2843,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2826,7 +2854,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2837,7 +2865,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2848,7 +2876,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2859,7 +2887,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2870,7 +2898,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2881,7 +2909,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2892,7 +2920,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2903,7 +2931,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2914,7 +2942,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2925,7 +2953,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2936,7 +2964,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2947,7 +2975,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2958,7 +2986,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2969,7 +2997,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2980,7 +3008,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2991,7 +3019,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3002,7 +3030,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3013,7 +3041,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3024,7 +3052,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3035,7 +3063,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3046,7 +3074,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3057,7 +3085,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3068,7 +3096,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3079,7 +3107,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3090,7 +3118,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3101,7 +3129,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3112,7 +3140,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3123,7 +3151,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3134,7 +3162,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3145,7 +3173,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3156,7 +3184,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3167,7 +3195,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3178,7 +3206,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3189,7 +3217,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3200,7 +3228,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3211,7 +3239,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3222,7 +3250,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3233,7 +3261,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3244,7 +3272,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3255,7 +3283,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3266,7 +3294,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3277,7 +3305,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3288,7 +3316,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3299,7 +3327,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3310,7 +3338,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3321,7 +3349,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3332,7 +3360,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3343,7 +3371,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3354,7 +3382,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3365,7 +3393,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3376,7 +3404,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3387,7 +3415,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3398,7 +3426,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3409,7 +3437,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3420,7 +3448,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3431,7 +3459,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3442,7 +3470,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3453,7 +3481,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3464,7 +3492,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3475,7 +3503,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3486,7 +3514,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3497,7 +3525,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3508,7 +3536,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3519,7 +3547,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3530,7 +3558,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3541,7 +3569,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3552,7 +3580,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3563,7 +3591,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3574,7 +3602,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3585,7 +3613,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3596,7 +3624,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3607,7 +3635,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3618,7 +3646,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3629,7 +3657,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3640,7 +3668,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3651,7 +3679,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3662,7 +3690,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3673,7 +3701,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3684,7 +3712,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3695,7 +3723,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3706,7 +3734,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3717,7 +3745,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3728,7 +3756,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3739,7 +3767,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3750,7 +3778,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3761,7 +3789,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3772,7 +3800,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3783,7 +3811,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3794,7 +3822,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3805,7 +3833,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3816,7 +3844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3827,7 +3855,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3838,7 +3866,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3849,7 +3877,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3860,7 +3888,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3871,7 +3899,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3882,7 +3910,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3893,7 +3921,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3904,7 +3932,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="2"/>
@@ -3915,7 +3943,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C186" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 79: Net Returns UI
Net Returns UI with cashflows and summary grid
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpol\ArkWeb\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchaturvedi\Repo\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130AEB6C-97A3-41CB-B938-6B6B40A84036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kC8cM+8NKgfNlXVeoq5zl6JRNnNR9PO0G60Jdw7TqaTbfLSEZ9nK8EFdniUSnnBb1qczKmXNKtSwprRxwcyB+A==" workbookSaltValue="zEbgma0RL1csL60XTK2z4w==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A926C0-CA46-4EFA-8732-33526317CBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="6dh46PIWWM4eNLbrHIgXqVj04c03dUHTzzKy1Y/ReG8TuFaAwA+9lb6mFFrYEpzeCyF5G6TDtyApGp8LLtLhuA==" workbookSaltValue="ZoQ4KgNSZp+C3CNuK1DeLA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12336" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="265">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -816,6 +816,21 @@
   </si>
   <si>
     <t>SMA HAIL HSBC</t>
+  </si>
+  <si>
+    <t>Deferred loan origination fee income</t>
+  </si>
+  <si>
+    <t>Current quarter rebates</t>
+  </si>
+  <si>
+    <t>Organisational costs unamortised</t>
+  </si>
+  <si>
+    <t>Opex</t>
+  </si>
+  <si>
+    <t>Setup costs</t>
   </si>
 </sst>
 </file>
@@ -1359,7 +1374,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,7 +1445,9 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="22"/>
+      <c r="I2" s="22" t="s">
+        <v>213</v>
+      </c>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
@@ -1602,7 +1619,7 @@
       <c r="M13" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3TB3pj9S0mk47Ql/h8d/p4vhDYOoLbG6vyzq/HY/4/08ku3fLQtKQeiK2aTRZt4jZdmX6a2/EM9TdwOYmGbvRA==" saltValue="E4Hx5yIm54bcuKuwmcoj2Q==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ciKEeOvnYy+G7HYzzQw4uq2ZnJ3qQdPrc4j4SIOSjHzFvmLqEtZEVFkc7XdwitJmsRGp/LDhOEiBAaQR/S85pw==" saltValue="CWtpmIMeYMU47VGAffWajw==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1630,7 +1647,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$C$1:$C$19</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>J3:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{85863E50-D527-4AC5-A2D8-C6D4BC7E5ACE}">
           <x14:formula1>
@@ -1648,7 +1665,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$4:$A$56</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C5 C7:C1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00ECCC13-F8BB-4BC7-9E76-CE6657AC06A8}">
           <x14:formula1>
@@ -1662,11 +1679,11 @@
           </x14:formula1>
           <xm:sqref>G1 G2:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BB1976F-BBF5-4D73-BB5B-CEA6D4D39945}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B13AF546-7D9A-44B6-BECE-72F315E7DD2B}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$4:$A$56</xm:f>
+            <xm:f>IF($I$2="NAV",Sheet2!$C$20:$C$29,Sheet2!$C$1:$C$24)</xm:f>
           </x14:formula1>
-          <xm:sqref>C6</xm:sqref>
+          <xm:sqref>J2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1679,8 +1696,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J186"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2048,7 +2065,9 @@
         <v>22</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="D20" s="2">
         <v>176</v>
       </c>
@@ -2061,7 +2080,9 @@
         <v>23</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>261</v>
+      </c>
       <c r="D21" s="2">
         <v>181</v>
       </c>
@@ -2074,7 +2095,9 @@
         <v>24</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>262</v>
+      </c>
       <c r="D22" s="2">
         <v>182</v>
       </c>
@@ -2087,7 +2110,9 @@
         <v>25</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="D23" s="2">
         <v>183</v>
       </c>
@@ -2100,7 +2125,9 @@
         <v>26</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>264</v>
+      </c>
       <c r="D24" s="2">
         <v>200</v>
       </c>
@@ -2113,7 +2140,9 @@
         <v>27</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="D25" s="2">
         <v>202</v>
       </c>
@@ -2126,7 +2155,9 @@
         <v>28</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>219</v>
+      </c>
       <c r="D26" s="2">
         <v>205</v>
       </c>
@@ -2139,7 +2170,9 @@
         <v>29</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="D27" s="2">
         <v>206</v>
       </c>
@@ -2152,7 +2185,9 @@
         <v>30</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="D28" s="2">
         <v>208</v>
       </c>
@@ -2165,7 +2200,9 @@
         <v>31</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>220</v>
+      </c>
       <c r="D29" s="2">
         <v>215</v>
       </c>

</xml_diff>

<commit_message>
AC-291. Setting SL2FEUR as default fundhedging
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,13 +5,13 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchaturvedi\Repo\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchaturvedi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A926C0-CA46-4EFA-8732-33526317CBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192BFB4E-6313-4229-9DC1-EF2F0C8F8F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="6dh46PIWWM4eNLbrHIgXqVj04c03dUHTzzKy1Y/ReG8TuFaAwA+9lb6mFFrYEpzeCyF5G6TDtyApGp8LLtLhuA==" workbookSaltValue="ZoQ4KgNSZp+C3CNuK1DeLA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12336" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="12360" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="265">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -1374,7 +1374,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1445,9 +1445,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="22" t="s">
-        <v>213</v>
-      </c>
+      <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>

</xml_diff>

<commit_message>
Merged PR 113: AC-291| Changed Net Returns summary column order
- AC-291| Changed Net Returns summary column order
- AC-291| Changed column order and name
- Merge branch 'main' into AC-291
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchaturvedi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192BFB4E-6313-4229-9DC1-EF2F0C8F8F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="6dh46PIWWM4eNLbrHIgXqVj04c03dUHTzzKy1Y/ReG8TuFaAwA+9lb6mFFrYEpzeCyF5G6TDtyApGp8LLtLhuA==" workbookSaltValue="ZoQ4KgNSZp+C3CNuK1DeLA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C2A49F-3ADC-4AAE-965D-899C6F6E34EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="JfWcpnUIhB7/jJfthg5ITHCPO5lI5mNxgtC8yh5I6BhBW80mwtlwglCgYaXs8VLA0Iq43CiBBpiuDugzrKvZ/Q==" workbookSaltValue="x9uw3C9kmQMq7ylVRd1MRA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="384" windowWidth="23040" windowHeight="12360" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="266">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -831,6 +831,9 @@
   </si>
   <si>
     <t>Setup costs</t>
+  </si>
+  <si>
+    <t>Deferred credit facility costs</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1383,7 @@
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="22" bestFit="1" customWidth="1"/>
@@ -1617,7 +1620,7 @@
       <c r="M13" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ciKEeOvnYy+G7HYzzQw4uq2ZnJ3qQdPrc4j4SIOSjHzFvmLqEtZEVFkc7XdwitJmsRGp/LDhOEiBAaQR/S85pw==" saltValue="CWtpmIMeYMU47VGAffWajw==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="RMp9q0USHBXgTdch4C+RQSKD7WImeb5n3tO9VHAUhC+LfSBOPxn/CKMGaspSxzD5Sdtgc92cW71OuQxp7wpASg==" saltValue="o731s2QD3J/iqJVxVmSYuw==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1679,7 +1682,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B13AF546-7D9A-44B6-BECE-72F315E7DD2B}">
           <x14:formula1>
-            <xm:f>IF($I$2="NAV",Sheet2!$C$20:$C$29,Sheet2!$C$1:$C$24)</xm:f>
+            <xm:f>IF($I$2="NAV",Sheet2!$C$22:$C$31,Sheet2!$C$1:$C$31)</xm:f>
           </x14:formula1>
           <xm:sqref>J2</xm:sqref>
         </x14:dataValidation>
@@ -1695,7 +1698,7 @@
   <dimension ref="A1:J186"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2064,7 +2067,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D20" s="2">
         <v>176</v>
@@ -2079,7 +2082,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D21" s="2">
         <v>181</v>
@@ -2094,7 +2097,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D22" s="2">
         <v>182</v>
@@ -2109,7 +2112,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D23" s="2">
         <v>183</v>
@@ -2124,7 +2127,7 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D24" s="2">
         <v>200</v>
@@ -2213,7 +2216,9 @@
         <v>32</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="D30" s="2">
         <v>216</v>
       </c>
@@ -2226,7 +2231,9 @@
         <v>33</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="C31" s="17" t="s">
+        <v>265</v>
+      </c>
       <c r="D31" s="2">
         <v>218</v>
       </c>
@@ -2239,7 +2246,6 @@
         <v>34</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
       <c r="D32" s="2">
         <v>219</v>
       </c>

</xml_diff>

<commit_message>
Added new Capital Subtype in template file
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchaturvedi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dchaturvedi\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C2A49F-3ADC-4AAE-965D-899C6F6E34EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="JfWcpnUIhB7/jJfthg5ITHCPO5lI5mNxgtC8yh5I6BhBW80mwtlwglCgYaXs8VLA0Iq43CiBBpiuDugzrKvZ/Q==" workbookSaltValue="x9uw3C9kmQMq7ylVRd1MRA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBED945-5D32-45FD-A376-5B00BF0E6322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="QkOhL8kZpUFFvgncwAyD8k/7/CWxAuBuCKq8Ku+2j5bU0PCVFEGPZqauAHK0RsH7v4VEmFwg8JjX0aRU5G7qJg==" workbookSaltValue="kczNB/iy5ROABBee31lMKw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="267">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -834,6 +834,9 @@
   </si>
   <si>
     <t>Deferred credit facility costs</t>
+  </si>
+  <si>
+    <t>Subscription costs unamortised</t>
   </si>
 </sst>
 </file>
@@ -1620,7 +1623,7 @@
       <c r="M13" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="RMp9q0USHBXgTdch4C+RQSKD7WImeb5n3tO9VHAUhC+LfSBOPxn/CKMGaspSxzD5Sdtgc92cW71OuQxp7wpASg==" saltValue="o731s2QD3J/iqJVxVmSYuw==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="lve7BvsLO7AaYQXzu2WdXI0LllIFIIWWcpqZub6Wmwp1sy+BBVnViWCBKBD7naQxCtjCwp5CihNtTEeqVLaEaQ==" saltValue="ZEmP6dlMUQyuOnPIqY4uJg==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1682,7 +1685,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B13AF546-7D9A-44B6-BECE-72F315E7DD2B}">
           <x14:formula1>
-            <xm:f>IF($I$2="NAV",Sheet2!$C$22:$C$31,Sheet2!$C$1:$C$31)</xm:f>
+            <xm:f>IF($I$2="NAV",Sheet2!$C$22:$C$32,Sheet2!$C$1:$C$32)</xm:f>
           </x14:formula1>
           <xm:sqref>J2</xm:sqref>
         </x14:dataValidation>
@@ -1697,8 +1700,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J186"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2246,6 +2249,9 @@
         <v>34</v>
       </c>
       <c r="B32" s="2"/>
+      <c r="C32" s="17" t="s">
+        <v>266</v>
+      </c>
       <c r="D32" s="2">
         <v>219</v>
       </c>

</xml_diff>

<commit_message>
Merged PR 197: AC-349 | Removing Performance fee paid from NAV quarterly template
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC23FBEA-145A-40E1-B105-DA6949E31DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="EVEWNv0v88C68wpmjQ5drBqTDo/0c2wHkTSOpwPthTu0517m/PpOp6puBVoLJgbxso9GtJH1A+KkrHj3nHT0ZQ==" workbookSaltValue="1bYLzaZNf4/km08HZaWdUA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDE81B9-F782-41D1-98C0-1A5034625EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2475" windowWidth="24240" windowHeight="13020" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="274">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -857,6 +857,9 @@
   </si>
   <si>
     <t>IU Group</t>
+  </si>
+  <si>
+    <t>Performance fee paid</t>
   </si>
 </sst>
 </file>
@@ -890,7 +893,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -912,6 +915,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAEAAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1038,7 +1047,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1078,6 +1087,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,22 +1410,22 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1447,7 +1457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="19"/>
@@ -1459,7 +1469,7 @@
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
     </row>
-    <row r="3" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="19"/>
@@ -1471,7 +1481,7 @@
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
     </row>
-    <row r="4" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="19"/>
@@ -1483,7 +1493,7 @@
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
     </row>
-    <row r="5" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="19"/>
@@ -1495,7 +1505,7 @@
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
     </row>
-    <row r="6" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="19"/>
@@ -1507,7 +1517,7 @@
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
     </row>
-    <row r="7" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="19"/>
@@ -1519,7 +1529,7 @@
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
     </row>
-    <row r="8" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="19"/>
@@ -1531,7 +1541,7 @@
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
     </row>
-    <row r="9" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="19"/>
@@ -1543,7 +1553,7 @@
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
     </row>
-    <row r="10" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="19"/>
@@ -1555,7 +1565,7 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
     </row>
-    <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="19"/>
@@ -1567,7 +1577,7 @@
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
     </row>
-    <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="19"/>
@@ -1579,7 +1589,7 @@
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
     </row>
-    <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="19"/>
@@ -1592,7 +1602,7 @@
       <c r="J13" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MchCAHC0YYomvH8iEms8dDvOR6zL6AQeB7teYmV1Ic0LSczH3mf5Aj9QMjJM8R4WzEEPYi+HaufDPkLQfKL+tQ==" saltValue="djAifgQ41imehIytBoTkqQ==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dq+n9hQJDWBQrzFrQ+hlsa4z2QLGRUrdeSlF4vwKCJ573238R7KFPFo1sRdfrt+LWSp/OrUuw5gx9zzbD/F2zQ==" saltValue="sXL+Lr9FPHHYk1LirZI1Nw==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1612,13 +1622,7 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99270DBF-3797-4B62-BFCE-7F002DF50F56}">
-          <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$19</xm:f>
-          </x14:formula1>
-          <xm:sqref>G3:G1048576</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD33D8DB-60D7-4F0B-971A-5F8F33CA4B56}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
@@ -1637,11 +1641,11 @@
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B13AF546-7D9A-44B6-BECE-72F315E7DD2B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{75DFCCCF-5BF2-4AC4-9BAC-3C15AF6DFB99}">
           <x14:formula1>
-            <xm:f>IF($F$2="NAV",Sheet2!$C$22:$C$32,Sheet2!$C$1:$C$32)</xm:f>
+            <xm:f>IF($F2="NAV",Sheet2!$C$22:$C$33,Sheet2!$C$1:$C$33)</xm:f>
           </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1654,21 +1658,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J186"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1694,7 +1698,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1743,7 +1747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1766,7 +1770,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
@@ -1789,7 +1793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1807,7 +1811,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1825,7 +1829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1843,7 +1847,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -1861,7 +1865,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>52</v>
       </c>
@@ -1879,7 +1883,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1894,7 +1898,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1909,7 +1913,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
@@ -1924,7 +1928,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
@@ -1939,7 +1943,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
@@ -1954,7 +1958,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
@@ -1969,7 +1973,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>70</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>73</v>
       </c>
@@ -1999,7 +2003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
@@ -2014,7 +2018,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -2029,7 +2033,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
@@ -2044,12 +2048,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D22" s="2">
@@ -2059,12 +2063,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="21" t="s">
         <v>88</v>
       </c>
       <c r="D23" s="2">
@@ -2074,12 +2078,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="21" t="s">
         <v>90</v>
       </c>
       <c r="D24" s="2">
@@ -2089,12 +2093,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="21" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="2">
@@ -2104,12 +2108,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="21" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="2">
@@ -2119,12 +2123,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="21" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="2">
@@ -2134,12 +2138,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="21" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="2">
@@ -2149,12 +2153,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="2">
@@ -2164,12 +2168,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="21" t="s">
         <v>62</v>
       </c>
       <c r="D30" s="2">
@@ -2179,12 +2183,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="21" t="s">
         <v>105</v>
       </c>
       <c r="D31" s="2">
@@ -2194,12 +2198,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="21" t="s">
         <v>108</v>
       </c>
       <c r="D32" s="2">
@@ -2209,12 +2213,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>110</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="C33" s="21" t="s">
+        <v>273</v>
+      </c>
       <c r="D33" s="2">
         <v>220</v>
       </c>
@@ -2222,7 +2228,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>112</v>
       </c>
@@ -2235,7 +2241,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>114</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>116</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>118</v>
       </c>
@@ -2274,7 +2280,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>120</v>
       </c>
@@ -2287,7 +2293,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>122</v>
       </c>
@@ -2300,7 +2306,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>124</v>
       </c>
@@ -2313,7 +2319,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
         <v>126</v>
       </c>
@@ -2326,7 +2332,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="s">
         <v>128</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
         <v>130</v>
       </c>
@@ -2352,7 +2358,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
         <v>132</v>
       </c>
@@ -2365,7 +2371,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
         <v>134</v>
       </c>
@@ -2378,7 +2384,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
         <v>136</v>
       </c>
@@ -2391,7 +2397,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>138</v>
       </c>
@@ -2404,7 +2410,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>139</v>
       </c>
@@ -2417,7 +2423,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
         <v>141</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
         <v>143</v>
       </c>
@@ -2443,7 +2449,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
         <v>145</v>
       </c>
@@ -2456,7 +2462,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>149</v>
       </c>
@@ -2482,7 +2488,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>151</v>
       </c>
@@ -2495,7 +2501,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>153</v>
       </c>
@@ -2508,7 +2514,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>155</v>
       </c>
@@ -2521,7 +2527,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>157</v>
       </c>
@@ -2534,7 +2540,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>158</v>
       </c>
@@ -2547,7 +2553,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>160</v>
       </c>
@@ -2560,7 +2566,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>162</v>
       </c>
@@ -2573,7 +2579,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>164</v>
       </c>
@@ -2586,7 +2592,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>166</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>167</v>
       </c>
@@ -2612,7 +2618,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>169</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>171</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2649,7 +2655,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2660,7 +2666,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2671,7 +2677,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2682,7 +2688,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2693,7 +2699,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2704,7 +2710,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2715,7 +2721,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2726,7 +2732,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2737,7 +2743,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2748,7 +2754,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2759,7 +2765,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2770,7 +2776,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2781,7 +2787,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2792,7 +2798,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2803,7 +2809,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2814,7 +2820,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2825,7 +2831,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2836,7 +2842,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2847,7 +2853,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2858,7 +2864,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2869,7 +2875,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2880,7 +2886,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2891,7 +2897,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2902,7 +2908,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2913,7 +2919,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2924,7 +2930,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2935,7 +2941,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2946,7 +2952,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2957,7 +2963,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2968,7 +2974,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2979,7 +2985,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2990,7 +2996,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3001,7 +3007,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3012,7 +3018,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3023,7 +3029,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3034,7 +3040,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3045,7 +3051,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3056,7 +3062,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3067,7 +3073,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3078,7 +3084,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3089,7 +3095,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3100,7 +3106,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3111,7 +3117,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3122,7 +3128,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3133,7 +3139,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3144,7 +3150,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3155,7 +3161,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3166,7 +3172,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3177,7 +3183,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3188,7 +3194,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3199,7 +3205,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3210,7 +3216,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3221,7 +3227,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3232,7 +3238,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3243,7 +3249,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3254,7 +3260,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3265,7 +3271,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3276,7 +3282,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3287,7 +3293,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3298,7 +3304,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3309,7 +3315,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3320,7 +3326,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3331,7 +3337,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3342,7 +3348,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3353,7 +3359,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3364,7 +3370,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3375,7 +3381,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3386,7 +3392,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3397,7 +3403,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3408,7 +3414,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3419,7 +3425,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3430,7 +3436,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3441,7 +3447,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3452,7 +3458,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3463,7 +3469,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3474,7 +3480,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3485,7 +3491,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3496,7 +3502,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3507,7 +3513,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3518,7 +3524,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3529,7 +3535,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3540,7 +3546,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3551,7 +3557,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3562,7 +3568,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3573,7 +3579,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3584,7 +3590,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3595,7 +3601,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3606,7 +3612,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3617,7 +3623,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3628,7 +3634,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3639,7 +3645,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3650,7 +3656,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3661,7 +3667,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3672,7 +3678,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3683,7 +3689,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3694,7 +3700,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3705,7 +3711,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3716,7 +3722,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3727,7 +3733,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3738,7 +3744,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3749,7 +3755,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3760,7 +3766,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3771,7 +3777,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3782,7 +3788,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3793,7 +3799,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3804,7 +3810,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3815,7 +3821,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3826,7 +3832,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3837,7 +3843,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3848,7 +3854,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3859,7 +3865,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3870,7 +3876,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3881,7 +3887,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3892,7 +3898,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3903,7 +3909,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3914,7 +3920,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3925,7 +3931,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3936,7 +3942,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3947,7 +3953,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="2"/>
@@ -3958,7 +3964,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C186" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 229: Strategy added to CA form, bulk and NAV quarterly upload templates
Strategy added to templates and on form.
Hiding Issuer fields on edit form load for NAV types
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,13 +5,13 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgosalia\source\repos\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDE81B9-F782-41D1-98C0-1A5034625EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7412F9B5-2265-4BAD-BA07-B42CD4176EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="MP5FdgzGrbJ11cOnDrUiPejm5u4H5XPu63a+IpBwBd0l3JDkOu59S1qdxiGrRL7Zm79y5SHushtKVeN/InBOrA==" workbookSaltValue="B6eySEDo8BojVQBKRocE7Q==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14490" windowHeight="7390" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="276">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -860,6 +860,12 @@
   </si>
   <si>
     <t>Performance fee paid</t>
+  </si>
+  <si>
+    <t>Co-Investments</t>
+  </si>
+  <si>
+    <t>Strategy/Currency</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1088,6 +1094,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1403,29 +1413,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AF4C19-D9D8-4D17-BA71-C91E169BA22D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="13.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.453125" style="19" customWidth="1"/>
+    <col min="12" max="16384" width="9.08984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1456,8 +1467,11 @@
       <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="19"/>
@@ -1468,8 +1482,9 @@
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
-    </row>
-    <row r="3" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="19"/>
@@ -1480,8 +1495,9 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
-    </row>
-    <row r="4" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="19"/>
@@ -1492,8 +1508,9 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
-    </row>
-    <row r="5" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="19"/>
@@ -1504,8 +1521,9 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
-    </row>
-    <row r="6" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="19"/>
@@ -1516,8 +1534,9 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
-    </row>
-    <row r="7" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="19"/>
@@ -1528,8 +1547,9 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="19"/>
@@ -1540,8 +1560,9 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="19"/>
@@ -1552,8 +1573,9 @@
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
-    </row>
-    <row r="10" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="19"/>
@@ -1564,8 +1586,9 @@
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
-    </row>
-    <row r="11" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="19"/>
@@ -1576,8 +1599,9 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
-    </row>
-    <row r="12" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="19"/>
@@ -1588,8 +1612,9 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="19"/>
@@ -1600,9 +1625,10 @@
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dq+n9hQJDWBQrzFrQ+hlsa4z2QLGRUrdeSlF4vwKCJ573238R7KFPFo1sRdfrt+LWSp/OrUuw5gx9zzbD/F2zQ==" saltValue="sXL+Lr9FPHHYk1LirZI1Nw==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Vi5HVqtyMexLSKLxlhNQX9vsNW0kvrosR4MpKqeRs2spNAVH2APnoF4URrtDwYX64yEyoMJjL0IVflLwu28xkw==" saltValue="PDgUpG3ZHnVW+VH1/Bgq5w==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1622,7 +1648,7 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD33D8DB-60D7-4F0B-971A-5F8F33CA4B56}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
@@ -1641,9 +1667,15 @@
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{75DFCCCF-5BF2-4AC4-9BAC-3C15AF6DFB99}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{19011AA8-B89A-470E-A9A0-4F39D1F83221}">
           <x14:formula1>
-            <xm:f>IF($F2="NAV",Sheet2!$C$22:$C$33,Sheet2!$C$1:$C$33)</xm:f>
+            <xm:f>Sheet2!$K$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B3D68DD-1FB2-428D-BC49-D4905BD3DB56}">
+          <x14:formula1>
+            <xm:f>IF($F2="NAV",Sheet2!$C$21:$C$33,Sheet2!$C$1:$C$33)</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
@@ -1656,23 +1688,24 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE38E7C1-F75A-461B-83D8-D3E941B09876}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J186"/>
+  <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1697,8 +1730,11 @@
       <c r="J1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1724,7 +1760,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1747,7 +1783,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1770,7 +1806,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
@@ -1793,7 +1829,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1811,7 +1847,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1829,7 +1865,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1847,7 +1883,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -1865,7 +1901,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>52</v>
       </c>
@@ -1883,7 +1919,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1898,7 +1934,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1913,7 +1949,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
@@ -1928,7 +1964,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
@@ -1943,13 +1979,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2">
         <v>130</v>
@@ -1958,13 +1994,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2">
         <v>141</v>
@@ -1973,13 +2009,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2">
         <v>142</v>
@@ -1988,13 +2024,13 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D18" s="2">
         <v>148</v>
@@ -2003,13 +2039,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D19" s="2">
         <v>158</v>
@@ -2018,13 +2054,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D20" s="2">
         <v>176</v>
@@ -2033,13 +2069,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>83</v>
+      <c r="C21" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="D21" s="2">
         <v>181</v>
@@ -2048,13 +2084,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2">
         <v>182</v>
@@ -2063,13 +2099,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2">
         <v>183</v>
@@ -2078,13 +2114,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="21" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="D24" s="2">
         <v>200</v>
@@ -2093,13 +2129,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="21" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D25" s="2">
         <v>202</v>
@@ -2108,13 +2144,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="21" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D26" s="2">
         <v>205</v>
@@ -2123,13 +2159,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D27" s="2">
         <v>206</v>
@@ -2138,13 +2174,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="21" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2">
         <v>208</v>
@@ -2153,13 +2189,13 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="21" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D29" s="2">
         <v>215</v>
@@ -2168,13 +2204,13 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="21" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="D30" s="2">
         <v>216</v>
@@ -2183,13 +2219,13 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="21" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D31" s="2">
         <v>218</v>
@@ -2198,13 +2234,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="21" t="s">
-        <v>108</v>
+        <v>273</v>
       </c>
       <c r="D32" s="2">
         <v>219</v>
@@ -2213,13 +2249,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>110</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="21" t="s">
-        <v>273</v>
+        <v>65</v>
       </c>
       <c r="D33" s="2">
         <v>220</v>
@@ -2228,7 +2264,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>112</v>
       </c>
@@ -2241,7 +2277,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>114</v>
       </c>
@@ -2254,7 +2290,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>116</v>
       </c>
@@ -2267,7 +2303,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>118</v>
       </c>
@@ -2280,7 +2316,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>120</v>
       </c>
@@ -2293,7 +2329,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>122</v>
       </c>
@@ -2306,7 +2342,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
         <v>124</v>
       </c>
@@ -2319,7 +2355,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="16" t="s">
         <v>126</v>
       </c>
@@ -2332,7 +2368,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="16" t="s">
         <v>128</v>
       </c>
@@ -2345,7 +2381,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="16" t="s">
         <v>130</v>
       </c>
@@ -2358,7 +2394,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="16" t="s">
         <v>132</v>
       </c>
@@ -2371,7 +2407,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="16" t="s">
         <v>134</v>
       </c>
@@ -2384,7 +2420,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="17" t="s">
         <v>136</v>
       </c>
@@ -2397,7 +2433,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="16" t="s">
         <v>138</v>
       </c>
@@ -2410,7 +2446,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="16" t="s">
         <v>139</v>
       </c>
@@ -2423,7 +2459,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="17" t="s">
         <v>141</v>
       </c>
@@ -2436,7 +2472,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="17" t="s">
         <v>143</v>
       </c>
@@ -2449,7 +2485,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="16" t="s">
         <v>145</v>
       </c>
@@ -2462,7 +2498,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -2475,7 +2511,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>149</v>
       </c>
@@ -2488,7 +2524,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>151</v>
       </c>
@@ -2501,7 +2537,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>153</v>
       </c>
@@ -2514,7 +2550,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>155</v>
       </c>
@@ -2527,7 +2563,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>157</v>
       </c>
@@ -2540,7 +2576,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>158</v>
       </c>
@@ -2553,7 +2589,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>160</v>
       </c>
@@ -2566,7 +2602,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>162</v>
       </c>
@@ -2579,7 +2615,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>164</v>
       </c>
@@ -2592,7 +2628,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>166</v>
       </c>
@@ -2605,7 +2641,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>167</v>
       </c>
@@ -2618,7 +2654,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>169</v>
       </c>
@@ -2631,7 +2667,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>171</v>
       </c>
@@ -2644,7 +2680,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2655,7 +2691,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2666,7 +2702,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2677,7 +2713,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2688,7 +2724,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2699,7 +2735,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2710,7 +2746,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2721,7 +2757,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2732,7 +2768,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2743,7 +2779,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2754,7 +2790,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2765,7 +2801,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2776,7 +2812,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2787,7 +2823,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2798,7 +2834,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2809,7 +2845,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2820,7 +2856,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2831,7 +2867,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2842,7 +2878,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2853,7 +2889,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2864,7 +2900,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2875,7 +2911,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2886,7 +2922,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2897,7 +2933,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2908,7 +2944,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2919,7 +2955,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2930,7 +2966,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2941,7 +2977,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2952,7 +2988,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2963,7 +2999,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2974,7 +3010,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2985,7 +3021,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2996,7 +3032,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3007,7 +3043,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3018,7 +3054,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3029,7 +3065,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3040,7 +3076,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3051,7 +3087,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3062,7 +3098,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3073,7 +3109,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3084,7 +3120,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3095,7 +3131,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3106,7 +3142,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3117,7 +3153,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3128,7 +3164,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3139,7 +3175,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3150,7 +3186,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3161,7 +3197,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3172,7 +3208,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3183,7 +3219,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3194,7 +3230,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3205,7 +3241,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3216,7 +3252,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3227,7 +3263,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3238,7 +3274,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3249,7 +3285,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3260,7 +3296,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3271,7 +3307,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3282,7 +3318,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3293,7 +3329,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3304,7 +3340,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3315,7 +3351,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3326,7 +3362,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3337,7 +3373,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3348,7 +3384,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3359,7 +3395,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3370,7 +3406,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3381,7 +3417,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3392,7 +3428,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3403,7 +3439,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3414,7 +3450,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3425,7 +3461,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3436,7 +3472,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3447,7 +3483,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3458,7 +3494,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3469,7 +3505,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3480,7 +3516,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3491,7 +3527,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3502,7 +3538,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3513,7 +3549,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3524,7 +3560,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3535,7 +3571,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3546,7 +3582,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3557,7 +3593,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3568,7 +3604,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3579,7 +3615,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3590,7 +3626,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3601,7 +3637,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3612,7 +3648,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3623,7 +3659,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3634,7 +3670,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3645,7 +3681,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3656,7 +3692,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3667,7 +3703,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3678,7 +3714,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3689,7 +3725,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3700,7 +3736,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3711,7 +3747,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3722,7 +3758,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3733,7 +3769,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3744,7 +3780,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3755,7 +3791,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3766,7 +3802,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3777,7 +3813,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3788,7 +3824,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3799,7 +3835,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3810,7 +3846,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3821,7 +3857,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3832,7 +3868,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3843,7 +3879,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3854,7 +3890,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3865,7 +3901,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3876,7 +3912,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3887,7 +3923,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3898,7 +3934,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3909,7 +3945,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -3920,7 +3956,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -3931,7 +3967,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -3942,7 +3978,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -3953,19 +3989,16 @@
         <v>271</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
-      <c r="C185" s="2"/>
+      <c r="C185" s="8"/>
       <c r="D185" s="8">
         <v>884</v>
       </c>
       <c r="E185" s="9" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C186" s="8"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G186">

</xml_diff>

<commit_message>
Merged PR 230: Added Strategy to Bulk Upload Templates and Investment Grid
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgosalia\source\repos\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7412F9B5-2265-4BAD-BA07-B42CD4176EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="MP5FdgzGrbJ11cOnDrUiPejm5u4H5XPu63a+IpBwBd0l3JDkOu59S1qdxiGrRL7Zm79y5SHushtKVeN/InBOrA==" workbookSaltValue="B6eySEDo8BojVQBKRocE7Q==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF5E875-9733-484D-B583-92643562621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="0BEtFWItXYVopYa4agcpRiE3VDIz0Wj7K8fzrotIw4A9JPIgxzdU/WoTYBslm2PeQYmFsq6C26Jr1mYHwmvGhQ==" workbookSaltValue="VcfmXPF9GY4riJOoxFwYCQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14490" windowHeight="7390" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="280">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -865,7 +866,19 @@
     <t>Co-Investments</t>
   </si>
   <si>
+    <t>Capsol</t>
+  </si>
+  <si>
     <t>Strategy/Currency</t>
+  </si>
+  <si>
+    <t>Finance Cost ITD</t>
+  </si>
+  <si>
+    <t>Net forward contract movements ITD (unrealised)</t>
+  </si>
+  <si>
+    <t>Net forward contract movements ITD (realised)</t>
   </si>
 </sst>
 </file>
@@ -876,7 +889,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -898,8 +911,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -928,6 +948,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1053,7 +1079,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1098,6 +1124,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1468,7 +1496,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
@@ -1628,7 +1656,7 @@
       <c r="K13" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Vi5HVqtyMexLSKLxlhNQX9vsNW0kvrosR4MpKqeRs2spNAVH2APnoF4URrtDwYX64yEyoMJjL0IVflLwu28xkw==" saltValue="PDgUpG3ZHnVW+VH1/Bgq5w==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wko311q4uLvdBv1L19A4gZ3RUmng8hR1pP0zincKmXTGnnCr6WC+DE6Skn1Qc+ia2oAwboIV5+GAkCFWu5SH3w==" saltValue="NJR+aJxXKL1EY9zPVA5RLQ==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1667,17 +1695,17 @@
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{19011AA8-B89A-470E-A9A0-4F39D1F83221}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B3D68DD-1FB2-428D-BC49-D4905BD3DB56}">
           <x14:formula1>
-            <xm:f>Sheet2!$K$1</xm:f>
+            <xm:f>IF($F2="NAV",Sheet2!$C$21:$C$36,Sheet2!$C$1:$C$36)</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CC864D65-DEB0-4BF6-B3D9-08B4A4FBCF3D}">
+          <x14:formula1>
+            <xm:f>Sheet2!$K$1:$K$5</xm:f>
           </x14:formula1>
           <xm:sqref>K2:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B3D68DD-1FB2-428D-BC49-D4905BD3DB56}">
-          <x14:formula1>
-            <xm:f>IF($F2="NAV",Sheet2!$C$21:$C$33,Sheet2!$C$1:$C$33)</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1690,8 +1718,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1759,6 +1787,9 @@
       <c r="J2" t="s">
         <v>23</v>
       </c>
+      <c r="K2" s="23" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
@@ -1782,6 +1813,9 @@
       <c r="I3" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="K3" s="23" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
@@ -1805,6 +1839,9 @@
       <c r="I4" s="10" t="s">
         <v>35</v>
       </c>
+      <c r="K4" s="23" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
@@ -1828,6 +1865,9 @@
       <c r="I5" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="K5" s="23" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
@@ -2269,7 +2309,9 @@
         <v>112</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="C34" s="24" t="s">
+        <v>277</v>
+      </c>
       <c r="D34" s="2">
         <v>221</v>
       </c>
@@ -2282,7 +2324,9 @@
         <v>114</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="C35" s="25" t="s">
+        <v>278</v>
+      </c>
       <c r="D35" s="2">
         <v>228</v>
       </c>
@@ -2295,7 +2339,9 @@
         <v>116</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="C36" s="25" t="s">
+        <v>279</v>
+      </c>
       <c r="D36" s="2">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
Added MinLinkedDate field and CA Bulk upload template changes for adding 2 new subtypes
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgosalia\source\repos\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\Desktop\AC-374\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF5E875-9733-484D-B583-92643562621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="0BEtFWItXYVopYa4agcpRiE3VDIz0Wj7K8fzrotIw4A9JPIgxzdU/WoTYBslm2PeQYmFsq6C26Jr1mYHwmvGhQ==" workbookSaltValue="VcfmXPF9GY4riJOoxFwYCQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC73E04-C8ED-46B9-9A73-58E680FB9BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Ryzqtsd+hcqVO/HMMWJ+VtTXEVT9caPT0lF7UXD2vpDMHldsSkiddrFYjbLfEe30LYfSPNDrPa4XjR1c+5CkQQ==" workbookSaltValue="lBH1IuoRfAHk/NLb5M++mQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="282">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -879,6 +878,12 @@
   </si>
   <si>
     <t>Net forward contract movements ITD (realised)</t>
+  </si>
+  <si>
+    <t>Total Operating exp (excluded GPS) ITD</t>
+  </si>
+  <si>
+    <t>Total foreign exchange movements ITD</t>
   </si>
 </sst>
 </file>
@@ -1445,26 +1450,26 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6328125" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="9.08984375" style="2"/>
+    <col min="1" max="1" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5546875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" style="19" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1499,7 +1504,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="19"/>
@@ -1512,7 +1517,7 @@
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
     </row>
-    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="19"/>
@@ -1525,7 +1530,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
     </row>
-    <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="19"/>
@@ -1538,7 +1543,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
     </row>
-    <row r="5" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="19"/>
@@ -1551,7 +1556,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
     </row>
-    <row r="6" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="19"/>
@@ -1564,7 +1569,7 @@
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="19"/>
@@ -1577,7 +1582,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
     </row>
-    <row r="8" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="19"/>
@@ -1590,7 +1595,7 @@
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
     </row>
-    <row r="9" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="19"/>
@@ -1603,7 +1608,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
     </row>
-    <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="19"/>
@@ -1616,7 +1621,7 @@
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="19"/>
@@ -1629,7 +1634,7 @@
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
     </row>
-    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="19"/>
@@ -1642,7 +1647,7 @@
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
     </row>
-    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="19"/>
@@ -1656,7 +1661,7 @@
       <c r="K13" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wko311q4uLvdBv1L19A4gZ3RUmng8hR1pP0zincKmXTGnnCr6WC+DE6Skn1Qc+ia2oAwboIV5+GAkCFWu5SH3w==" saltValue="NJR+aJxXKL1EY9zPVA5RLQ==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+CU3BAcheiDswhwZIcvqMb/Dp47kUUJrfqMAviHVOnwPGMzPi98a51GVFxWsNLAP6PMl02NMoHCP0UZY2pKtkw==" saltValue="jroZ/xcmcqrlA+RvkPg5jQ==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1697,7 +1702,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B3D68DD-1FB2-428D-BC49-D4905BD3DB56}">
           <x14:formula1>
-            <xm:f>IF($F2="NAV",Sheet2!$C$21:$C$36,Sheet2!$C$1:$C$36)</xm:f>
+            <xm:f>IF($F2="NAV",Sheet2!$C$21:$C$38,Sheet2!$C$1:$C$38)</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
@@ -1718,22 +1723,22 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" customWidth="1"/>
-    <col min="2" max="2" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1762,7 +1767,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1791,7 +1796,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1817,7 +1822,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1843,7 +1848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
@@ -1869,7 +1874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1887,7 +1892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1905,7 +1910,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1923,7 +1928,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -1941,7 +1946,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>52</v>
       </c>
@@ -1959,7 +1964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1974,7 +1979,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -1989,7 +1994,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
@@ -2004,7 +2009,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
@@ -2019,7 +2024,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
@@ -2034,7 +2039,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
@@ -2049,7 +2054,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>70</v>
       </c>
@@ -2064,7 +2069,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>73</v>
       </c>
@@ -2079,7 +2084,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>76</v>
       </c>
@@ -2094,7 +2099,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>79</v>
       </c>
@@ -2109,7 +2114,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
@@ -2124,7 +2129,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>85</v>
       </c>
@@ -2139,7 +2144,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -2154,7 +2159,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -2169,7 +2174,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>92</v>
       </c>
@@ -2184,7 +2189,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>94</v>
       </c>
@@ -2199,7 +2204,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>96</v>
       </c>
@@ -2214,7 +2219,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>98</v>
       </c>
@@ -2229,7 +2234,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>100</v>
       </c>
@@ -2244,7 +2249,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>102</v>
       </c>
@@ -2259,7 +2264,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>104</v>
       </c>
@@ -2274,7 +2279,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>107</v>
       </c>
@@ -2289,7 +2294,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>110</v>
       </c>
@@ -2304,7 +2309,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>112</v>
       </c>
@@ -2319,7 +2324,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>114</v>
       </c>
@@ -2334,7 +2339,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>116</v>
       </c>
@@ -2349,12 +2354,14 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="C37" s="25" t="s">
+        <v>281</v>
+      </c>
       <c r="D37" s="2">
         <v>249</v>
       </c>
@@ -2362,12 +2369,14 @@
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="C38" s="25" t="s">
+        <v>280</v>
+      </c>
       <c r="D38" s="2">
         <v>254</v>
       </c>
@@ -2375,7 +2384,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>122</v>
       </c>
@@ -2388,7 +2397,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>124</v>
       </c>
@@ -2401,7 +2410,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
         <v>126</v>
       </c>
@@ -2414,7 +2423,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="s">
         <v>128</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
         <v>130</v>
       </c>
@@ -2440,7 +2449,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
         <v>132</v>
       </c>
@@ -2453,7 +2462,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
         <v>134</v>
       </c>
@@ -2466,7 +2475,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
         <v>136</v>
       </c>
@@ -2479,7 +2488,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>138</v>
       </c>
@@ -2492,7 +2501,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>139</v>
       </c>
@@ -2505,7 +2514,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
         <v>141</v>
       </c>
@@ -2518,7 +2527,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
         <v>143</v>
       </c>
@@ -2531,7 +2540,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
         <v>145</v>
       </c>
@@ -2544,7 +2553,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>147</v>
       </c>
@@ -2557,7 +2566,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>149</v>
       </c>
@@ -2570,7 +2579,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>151</v>
       </c>
@@ -2583,7 +2592,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>153</v>
       </c>
@@ -2596,7 +2605,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>155</v>
       </c>
@@ -2609,7 +2618,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>157</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>158</v>
       </c>
@@ -2635,7 +2644,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>160</v>
       </c>
@@ -2648,7 +2657,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>162</v>
       </c>
@@ -2661,7 +2670,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>164</v>
       </c>
@@ -2674,7 +2683,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>166</v>
       </c>
@@ -2687,7 +2696,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>167</v>
       </c>
@@ -2700,7 +2709,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>169</v>
       </c>
@@ -2713,7 +2722,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>171</v>
       </c>
@@ -2726,7 +2735,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2737,7 +2746,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2748,7 +2757,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2759,7 +2768,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2770,7 +2779,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2781,7 +2790,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2792,7 +2801,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2803,7 +2812,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2814,7 +2823,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2825,7 +2834,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="5"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2836,7 +2845,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2847,7 +2856,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="5"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2858,7 +2867,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2869,7 +2878,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="5"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2880,7 +2889,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="5"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2891,7 +2900,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2902,7 +2911,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="5"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2913,7 +2922,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="5"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2924,7 +2933,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="5"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2935,7 +2944,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2946,7 +2955,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="5"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2957,7 +2966,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="5"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2968,7 +2977,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="5"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2979,7 +2988,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2990,7 +2999,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="5"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3001,7 +3010,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3012,7 +3021,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="5"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3023,7 +3032,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="5"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3034,7 +3043,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="5"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3045,7 +3054,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="5"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3056,7 +3065,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="5"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3067,7 +3076,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="5"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3078,7 +3087,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3089,7 +3098,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3100,7 +3109,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3111,7 +3120,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3122,7 +3131,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="5"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3133,7 +3142,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3144,7 +3153,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="5"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3155,7 +3164,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3166,7 +3175,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="5"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3177,7 +3186,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3188,7 +3197,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="5"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3199,7 +3208,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3210,7 +3219,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="5"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3221,7 +3230,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3232,7 +3241,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="5"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3243,7 +3252,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3254,7 +3263,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="5"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3265,7 +3274,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3276,7 +3285,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="5"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3287,7 +3296,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3298,7 +3307,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="5"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3309,7 +3318,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3320,7 +3329,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="5"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3331,7 +3340,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3342,7 +3351,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="5"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3353,7 +3362,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3364,7 +3373,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="5"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3375,7 +3384,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3386,7 +3395,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="5"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3397,7 +3406,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3408,7 +3417,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="5"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3419,7 +3428,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3430,7 +3439,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="5"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3441,7 +3450,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="5"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3452,7 +3461,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="5"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3463,7 +3472,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="5"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3474,7 +3483,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="5"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3485,7 +3494,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="5"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3496,7 +3505,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="5"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3507,7 +3516,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="5"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3518,7 +3527,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="5"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3529,7 +3538,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="5"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3540,7 +3549,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="5"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -3551,7 +3560,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="5"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -3562,7 +3571,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="5"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -3573,7 +3582,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="5"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -3584,7 +3593,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="5"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -3595,7 +3604,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="5"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -3606,7 +3615,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="5"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -3617,7 +3626,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="5"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -3628,7 +3637,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="5"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -3639,7 +3648,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="5"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -3650,7 +3659,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="5"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -3661,7 +3670,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="5"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -3672,7 +3681,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="5"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -3683,7 +3692,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="5"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -3694,7 +3703,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="5"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -3705,7 +3714,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="5"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -3716,7 +3725,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="5"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -3727,7 +3736,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="5"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -3738,7 +3747,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="5"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -3749,7 +3758,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="5"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -3760,7 +3769,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="5"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -3771,7 +3780,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="5"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -3782,7 +3791,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="5"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -3793,7 +3802,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="5"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -3804,7 +3813,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="5"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -3815,7 +3824,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="5"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -3826,7 +3835,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="5"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -3837,7 +3846,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="5"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -3848,7 +3857,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="5"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -3859,7 +3868,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="5"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -3870,7 +3879,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="5"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -3881,7 +3890,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -3892,7 +3901,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="5"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -3903,7 +3912,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="5"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -3914,7 +3923,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="5"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -3925,7 +3934,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="5"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -3936,7 +3945,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="5"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -3947,7 +3956,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="5"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -3958,7 +3967,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="5"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -3969,7 +3978,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="5"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -3980,7 +3989,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="5"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -3991,7 +4000,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="5"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -4002,7 +4011,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="5"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -4013,7 +4022,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="5"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -4024,7 +4033,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="5"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -4035,7 +4044,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="7"/>
       <c r="B185" s="8"/>
       <c r="C185" s="8"/>

</xml_diff>

<commit_message>
Splitting up Strategy/Currency fields in Capital Activity
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\Desktop\AC-374\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\source\repos\Ark-WebUI New\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC73E04-C8ED-46B9-9A73-58E680FB9BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Ryzqtsd+hcqVO/HMMWJ+VtTXEVT9caPT0lF7UXD2vpDMHldsSkiddrFYjbLfEe30LYfSPNDrPa4XjR1c+5CkQQ==" workbookSaltValue="lBH1IuoRfAHk/NLb5M++mQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01A9A84-5A36-4709-B825-855325BAAAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="XtcojnEd5zTVKzrbpyjvccIQJQs62l6EaDpXCe1HrgN2B+57J8KlTnVY/jfxRGMZx3bsfNXY0fghoINkVxDEpw==" workbookSaltValue="T3PHAtRvF7rGH+VnZp2csg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="283">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -868,9 +868,6 @@
     <t>Capsol</t>
   </si>
   <si>
-    <t>Strategy/Currency</t>
-  </si>
-  <si>
     <t>Finance Cost ITD</t>
   </si>
   <si>
@@ -884,6 +881,12 @@
   </si>
   <si>
     <t>Total foreign exchange movements ITD</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Override Currency</t>
   </si>
 </sst>
 </file>
@@ -1446,11 +1449,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AF4C19-D9D8-4D17-BA71-C91E169BA22D}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,11 +1468,11 @@
     <col min="8" max="8" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="2"/>
+    <col min="11" max="12" width="16.44140625" style="19" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1501,10 +1504,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="19"/>
@@ -1516,8 +1522,9 @@
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="19"/>
+    </row>
+    <row r="3" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="C3" s="19"/>
@@ -1529,8 +1536,9 @@
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
-    </row>
-    <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="19"/>
@@ -1542,8 +1550,9 @@
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="19"/>
@@ -1555,8 +1564,9 @@
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
-    </row>
-    <row r="6" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="19"/>
+    </row>
+    <row r="6" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="19"/>
@@ -1568,8 +1578,9 @@
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
-    </row>
-    <row r="7" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="19"/>
+    </row>
+    <row r="7" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="19"/>
@@ -1581,8 +1592,9 @@
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="19"/>
@@ -1594,8 +1606,9 @@
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
-    </row>
-    <row r="9" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="19"/>
@@ -1607,8 +1620,9 @@
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="19"/>
@@ -1620,8 +1634,9 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
-    </row>
-    <row r="11" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="19"/>
+    </row>
+    <row r="11" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
       <c r="C11" s="19"/>
@@ -1633,8 +1648,9 @@
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
-    </row>
-    <row r="12" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="19"/>
@@ -1646,8 +1662,9 @@
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
-    </row>
-    <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="19"/>
@@ -1659,9 +1676,10 @@
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+CU3BAcheiDswhwZIcvqMb/Dp47kUUJrfqMAviHVOnwPGMzPi98a51GVFxWsNLAP6PMl02NMoHCP0UZY2pKtkw==" saltValue="jroZ/xcmcqrlA+RvkPg5jQ==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="fD7kfTHy/DTyw2NtQCHED7gQ5FwS916XNyTQaH1ZNevibavEL3Iei5ywI2aOWmW/BLrejTpCM6LmUi/MA5VrNg==" saltValue="dxVfcWP6fygENpUA69Ym6w==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1698,7 +1716,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D1048576 L2:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B3D68DD-1FB2-428D-BC49-D4905BD3DB56}">
           <x14:formula1>
@@ -1708,9 +1726,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CC864D65-DEB0-4BF6-B3D9-08B4A4FBCF3D}">
           <x14:formula1>
-            <xm:f>Sheet2!$K$1:$K$5</xm:f>
+            <xm:f>Sheet2!$K$1:$K$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>K2:K1048542 K1048544:K1048576 K1048543</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1723,8 +1741,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1818,9 +1836,6 @@
       <c r="I3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="23" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1844,9 +1859,6 @@
       <c r="I4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1870,9 +1882,6 @@
       <c r="I5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="23" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -2315,7 +2324,7 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D34" s="2">
         <v>221</v>
@@ -2330,7 +2339,7 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D35" s="2">
         <v>228</v>
@@ -2345,7 +2354,7 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D36" s="2">
         <v>232</v>
@@ -2360,7 +2369,7 @@
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D37" s="2">
         <v>249</v>
@@ -2375,7 +2384,7 @@
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D38" s="2">
         <v>254</v>

</xml_diff>

<commit_message>
Added OverrideCurrency field validations
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,13 +5,13 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\source\repos\Ark-WebUI New\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\Documents\SQL Server Management Studio\AC-379\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01A9A84-5A36-4709-B825-855325BAAAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="XtcojnEd5zTVKzrbpyjvccIQJQs62l6EaDpXCe1HrgN2B+57J8KlTnVY/jfxRGMZx3bsfNXY0fghoINkVxDEpw==" workbookSaltValue="T3PHAtRvF7rGH+VnZp2csg==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2741A2-B2A7-48DA-8AD5-46B6774EBE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="j8Cb5VPbldlk2CYb7woyiywXYBfit+OzqbgZThUPWApicKCXZJHdYY1uskzz+QYoPn11Wk+xO653ZBrzr9JFog==" workbookSaltValue="xOkM5yh2V1mWIEjrmsbi1g==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="291">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -887,6 +887,30 @@
   </si>
   <si>
     <t>Override Currency</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>CIGNA</t>
+  </si>
+  <si>
+    <t>CS2FEUR</t>
+  </si>
+  <si>
+    <t>CS2FUSD</t>
+  </si>
+  <si>
+    <t>DL4COINV</t>
+  </si>
+  <si>
+    <t>DL4COINVEUR</t>
+  </si>
+  <si>
+    <t>SMA ILM</t>
+  </si>
+  <si>
+    <t>SMA SUMI</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1477,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1679,7 +1703,7 @@
       <c r="L13" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="fD7kfTHy/DTyw2NtQCHED7gQ5FwS916XNyTQaH1ZNevibavEL3Iei5ywI2aOWmW/BLrejTpCM6LmUi/MA5VrNg==" saltValue="dxVfcWP6fygENpUA69Ym6w==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="1J8nHOrkpjPmRWb1Zs7Ru1n2LRuScHiT1AJqwI2iIbypsVWGxx6YAWEcslkxSFOMAJa1pmb4JgZnwAj+Wu2EoA==" saltValue="zDKkviDAaKrD2CsiR7sPXg==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1699,7 +1723,7 @@
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD33D8DB-60D7-4F0B-971A-5F8F33CA4B56}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
@@ -1708,7 +1732,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BB1558C-DA49-446D-8D32-92277B04523E}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$4:$A$65</xm:f>
+            <xm:f>Sheet2!$A$4:$A$72</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -1716,7 +1740,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$G$1:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576 L2:L1048576</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4B3D68DD-1FB2-428D-BC49-D4905BD3DB56}">
           <x14:formula1>
@@ -1730,6 +1754,12 @@
           </x14:formula1>
           <xm:sqref>K2:K1048542 K1048544:K1048576 K1048543</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E9821568-F2B0-4280-A283-67B7B4AB7C8C}">
+          <x14:formula1>
+            <xm:f>Sheet2!$L$1:$L$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1739,10 +1769,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE38E7C1-F75A-461B-83D8-D3E941B09876}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K185"/>
+  <dimension ref="A1:L185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1756,7 +1786,7 @@
     <col min="12" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1784,8 +1814,11 @@
       <c r="K1" s="23" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -1813,8 +1846,11 @@
       <c r="K2" s="23" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1836,8 +1872,11 @@
       <c r="I3" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1859,8 +1898,11 @@
       <c r="I4" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
@@ -1882,8 +1924,11 @@
       <c r="I5" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1900,8 +1945,11 @@
       <c r="I6" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1918,8 +1966,11 @@
       <c r="I7" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="23" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>45</v>
       </c>
@@ -1937,7 +1988,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>48</v>
       </c>
@@ -1955,7 +2006,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>52</v>
       </c>
@@ -1973,7 +2024,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -1988,7 +2039,7 @@
         <v>40769165</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
@@ -2003,7 +2054,7 @@
         <v>27849185</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
@@ -2018,7 +2069,7 @@
         <v>10553774</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
@@ -2033,7 +2084,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>64</v>
       </c>
@@ -2048,7 +2099,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
@@ -2745,7 +2796,9 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
+      <c r="A66" s="5" t="s">
+        <v>284</v>
+      </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2">
@@ -2756,7 +2809,9 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
+      <c r="A67" s="5" t="s">
+        <v>285</v>
+      </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2">
@@ -2767,7 +2822,9 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
+      <c r="A68" s="5" t="s">
+        <v>286</v>
+      </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2">
@@ -2778,7 +2835,9 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
+      <c r="A69" s="5" t="s">
+        <v>287</v>
+      </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2">
@@ -2789,7 +2848,9 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
+      <c r="A70" s="5" t="s">
+        <v>288</v>
+      </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2">
@@ -2800,7 +2861,9 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="5"/>
+      <c r="A71" s="5" t="s">
+        <v>289</v>
+      </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2">
@@ -2811,7 +2874,9 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="5"/>
+      <c r="A72" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2">

</xml_diff>

<commit_message>
Added new Fund hedgings to template
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/CapitalActivityUploadTemplate.xlsx
@@ -5,13 +5,13 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\Desktop\AC-374\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\source\repos\Ark-WebUI New\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC73E04-C8ED-46B9-9A73-58E680FB9BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Ryzqtsd+hcqVO/HMMWJ+VtTXEVT9caPT0lF7UXD2vpDMHldsSkiddrFYjbLfEe30LYfSPNDrPa4XjR1c+5CkQQ==" workbookSaltValue="lBH1IuoRfAHk/NLb5M++mQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEA7837-52A9-4B05-B204-DE9B8759A3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="xEn5BfRxbXRzYNj8xrLIkEjYYIuzPbiW2VZA+uofOV68eROxGiB6vQRYv02cw5Hbr1VVzcUhYY8mnzyC9rnyTQ==" workbookSaltValue="raezSwHKAh+BU6qXyOEoHQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{39F0E884-8FC1-4CFB-8E7B-B66C412DCFC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalActivity" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="289">
   <si>
     <t>Cash Flow Date</t>
   </si>
@@ -884,6 +884,27 @@
   </si>
   <si>
     <t>Total foreign exchange movements ITD</t>
+  </si>
+  <si>
+    <t>CIGNA</t>
+  </si>
+  <si>
+    <t>CS2FEUR</t>
+  </si>
+  <si>
+    <t>CS2FUSD</t>
+  </si>
+  <si>
+    <t>DL4COINV</t>
+  </si>
+  <si>
+    <t>DL4COINVEUR</t>
+  </si>
+  <si>
+    <t>SMA ILM</t>
+  </si>
+  <si>
+    <t>SMA SUMI</t>
   </si>
 </sst>
 </file>
@@ -1450,7 +1471,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,7 +1682,7 @@
       <c r="K13" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+CU3BAcheiDswhwZIcvqMb/Dp47kUUJrfqMAviHVOnwPGMzPi98a51GVFxWsNLAP6PMl02NMoHCP0UZY2pKtkw==" saltValue="jroZ/xcmcqrlA+RvkPg5jQ==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/jBfzy1kZRylUbEHZ2Vb0WQXJHs1pNozjJGoF+RIG0OEYqtO1U0YMwies20hVK91C/3a/AvnYoE2hwHZOY43mA==" saltValue="uaoxcFzEu92cqLOZygxATQ==" spinCount="100000" sheet="1" formatColumns="0" formatRows="0"/>
   <dataValidations count="4">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{E83D86DC-2830-4F8A-AC13-16B156CBC213}">
       <formula1>42005</formula1>
@@ -1690,7 +1711,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8BB1558C-DA49-446D-8D32-92277B04523E}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$4:$A$65</xm:f>
+            <xm:f>Sheet2!$A$4:$A$72</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -1723,8 +1744,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2736,7 +2757,9 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
+      <c r="A66" s="5" t="s">
+        <v>282</v>
+      </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2">
@@ -2747,7 +2770,9 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
+      <c r="A67" s="5" t="s">
+        <v>283</v>
+      </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2">
@@ -2758,7 +2783,9 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
+      <c r="A68" s="5" t="s">
+        <v>284</v>
+      </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2">
@@ -2769,7 +2796,9 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
+      <c r="A69" s="5" t="s">
+        <v>285</v>
+      </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2">
@@ -2780,7 +2809,9 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
+      <c r="A70" s="5" t="s">
+        <v>286</v>
+      </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2">
@@ -2791,7 +2822,9 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="5"/>
+      <c r="A71" s="5" t="s">
+        <v>287</v>
+      </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2">
@@ -2802,7 +2835,9 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="5"/>
+      <c r="A72" s="5" t="s">
+        <v>288</v>
+      </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2">

</xml_diff>